<commit_message>
Lab 1 - finish
</commit_message>
<xml_diff>
--- a/lab4/1/bjt3.xlsx
+++ b/lab4/1/bjt3.xlsx
@@ -15,12 +15,12 @@
     <sheet name="B -voltage" sheetId="6" r:id="rId6"/>
     <sheet name="B - current" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>Run 1</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>diff</t>
+  </si>
+  <si>
+    <t>Transistor</t>
+  </si>
+  <si>
+    <t>Is</t>
   </si>
 </sst>
 </file>
@@ -6034,11 +6040,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73657728"/>
-        <c:axId val="73660032"/>
+        <c:axId val="546938880"/>
+        <c:axId val="546939456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73657728"/>
+        <c:axId val="546938880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6077,12 +6083,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73660032"/>
+        <c:crossAx val="546939456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73660032"/>
+        <c:axId val="546939456"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6127,7 +6133,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73657728"/>
+        <c:crossAx val="546938880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8799,11 +8805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73689920"/>
-        <c:axId val="74690496"/>
+        <c:axId val="546941760"/>
+        <c:axId val="546942336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73689920"/>
+        <c:axId val="546941760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8842,12 +8848,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74690496"/>
+        <c:crossAx val="546942336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74690496"/>
+        <c:axId val="546942336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.60000000000000009"/>
@@ -8888,7 +8894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73689920"/>
+        <c:crossAx val="546941760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10828,11 +10834,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="649355264"/>
-        <c:axId val="649337024"/>
+        <c:axId val="546944640"/>
+        <c:axId val="546945216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="649355264"/>
+        <c:axId val="546944640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10849,7 +10855,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Voltage (V)</a:t>
+                  <a:t>Base Voltage (V)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -10871,12 +10877,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649337024"/>
+        <c:crossAx val="546945216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="649337024"/>
+        <c:axId val="546945216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -10917,7 +10923,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649355264"/>
+        <c:crossAx val="546944640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10934,6 +10940,26 @@
       </c:legendEntry>
       <c:legendEntry>
         <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="7"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="9"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="10"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:layout/>
@@ -15576,11 +15602,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="633128064"/>
-        <c:axId val="633091712"/>
+        <c:axId val="548541504"/>
+        <c:axId val="548542080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="633128064"/>
+        <c:axId val="548541504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15624,12 +15650,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="633091712"/>
+        <c:crossAx val="548542080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="633091712"/>
+        <c:axId val="548542080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15669,7 +15695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="633128064"/>
+        <c:crossAx val="548541504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18418,11 +18444,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73657152"/>
-        <c:axId val="636206400"/>
+        <c:axId val="546947072"/>
+        <c:axId val="546947648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73657152"/>
+        <c:axId val="546947072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18466,12 +18492,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636206400"/>
+        <c:crossAx val="546947648"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="636206400"/>
+        <c:axId val="546947648"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -18512,7 +18538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73657152"/>
+        <c:crossAx val="546947072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18620,16 +18646,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -31789,7 +31815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V103"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
+    <sheetView topLeftCell="T7" workbookViewId="0">
       <selection activeCell="A2" sqref="A1:M1048576"/>
     </sheetView>
   </sheetViews>
@@ -36572,7 +36598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -36635,19 +36661,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="3">
-        <f>F3/$J3</f>
+        <f t="shared" ref="B3:B34" si="0">F3/$J3</f>
         <v>1.26984126984127</v>
       </c>
       <c r="C3" s="3">
-        <f>G3/$J3</f>
+        <f t="shared" ref="C3:C34" si="1">G3/$J3</f>
         <v>0.69841269841269848</v>
       </c>
       <c r="D3" s="3">
-        <f>H3/$J3</f>
+        <f t="shared" ref="D3:D34" si="2">H3/$J3</f>
         <v>0.69841269841269848</v>
       </c>
       <c r="E3" s="3">
-        <f>I3/$J3</f>
+        <f t="shared" ref="E3:E34" si="3">I3/$J3</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="F3" s="1">
@@ -36663,7 +36689,7 @@
         <v>2.0999999999999998E-9</v>
       </c>
       <c r="J3" s="1">
-        <f>AVERAGE(F3:I3)</f>
+        <f t="shared" ref="J3:J34" si="4">AVERAGE(F3:I3)</f>
         <v>1.5749999999999998E-9</v>
       </c>
     </row>
@@ -36672,19 +36698,19 @@
         <v>0.05</v>
       </c>
       <c r="B4" s="3">
-        <f>F4/$J4</f>
+        <f t="shared" si="0"/>
         <v>0.98285714285714287</v>
       </c>
       <c r="C4" s="3">
-        <f>G4/$J4</f>
+        <f t="shared" si="1"/>
         <v>0.96000000000000019</v>
       </c>
       <c r="D4" s="3">
-        <f>H4/$J4</f>
+        <f t="shared" si="2"/>
         <v>1.0857142857142859</v>
       </c>
       <c r="E4" s="3">
-        <f>I4/$J4</f>
+        <f t="shared" si="3"/>
         <v>0.97142857142857153</v>
       </c>
       <c r="F4" s="1">
@@ -36700,7 +36726,7 @@
         <v>-8.5E-9</v>
       </c>
       <c r="J4" s="1">
-        <f>AVERAGE(F4:I4)</f>
+        <f t="shared" si="4"/>
         <v>-8.7499999999999989E-9</v>
       </c>
     </row>
@@ -36709,19 +36735,19 @@
         <v>0.1</v>
       </c>
       <c r="B5" s="3">
-        <f>F5/$J5</f>
+        <f t="shared" si="0"/>
         <v>0.98245614035087714</v>
       </c>
       <c r="C5" s="3">
-        <f>G5/$J5</f>
+        <f t="shared" si="1"/>
         <v>0.92982456140350889</v>
       </c>
       <c r="D5" s="3">
-        <f>H5/$J5</f>
+        <f t="shared" si="2"/>
         <v>1.1754385964912279</v>
       </c>
       <c r="E5" s="3">
-        <f>I5/$J5</f>
+        <f t="shared" si="3"/>
         <v>0.91228070175438603</v>
       </c>
       <c r="F5" s="1">
@@ -36737,7 +36763,7 @@
         <v>-1.04E-8</v>
       </c>
       <c r="J5" s="1">
-        <f>AVERAGE(F5:I5)</f>
+        <f t="shared" si="4"/>
         <v>-1.14E-8</v>
       </c>
     </row>
@@ -36746,19 +36772,19 @@
         <v>0.15</v>
       </c>
       <c r="B6" s="3">
-        <f>F6/$J6</f>
+        <f t="shared" si="0"/>
         <v>0.89126559714795006</v>
       </c>
       <c r="C6" s="3">
-        <f>G6/$J6</f>
+        <f t="shared" si="1"/>
         <v>0.97682709447415317</v>
       </c>
       <c r="D6" s="3">
-        <f>H6/$J6</f>
+        <f t="shared" si="2"/>
         <v>1.1122994652406417</v>
       </c>
       <c r="E6" s="3">
-        <f>I6/$J6</f>
+        <f t="shared" si="3"/>
         <v>1.0196078431372548</v>
       </c>
       <c r="F6" s="1">
@@ -36774,7 +36800,7 @@
         <v>-1.4299999999999999E-8</v>
       </c>
       <c r="J6" s="1">
-        <f>AVERAGE(F6:I6)</f>
+        <f t="shared" si="4"/>
         <v>-1.4025000000000002E-8</v>
       </c>
     </row>
@@ -36783,19 +36809,19 @@
         <v>0.2</v>
       </c>
       <c r="B7" s="3">
-        <f>F7/$J7</f>
+        <f t="shared" si="0"/>
         <v>0.89696969696969719</v>
       </c>
       <c r="C7" s="3">
-        <f>G7/$J7</f>
+        <f t="shared" si="1"/>
         <v>0.90303030303030318</v>
       </c>
       <c r="D7" s="3">
-        <f>H7/$J7</f>
+        <f t="shared" si="2"/>
         <v>1.103030303030303</v>
       </c>
       <c r="E7" s="3">
-        <f>I7/$J7</f>
+        <f t="shared" si="3"/>
         <v>1.0969696969696972</v>
       </c>
       <c r="F7" s="1">
@@ -36811,7 +36837,7 @@
         <v>-1.81E-8</v>
       </c>
       <c r="J7" s="1">
-        <f>AVERAGE(F7:I7)</f>
+        <f t="shared" si="4"/>
         <v>-1.6499999999999999E-8</v>
       </c>
     </row>
@@ -36820,19 +36846,19 @@
         <v>0.25</v>
       </c>
       <c r="B8" s="3">
-        <f>F8/$J8</f>
+        <f t="shared" si="0"/>
         <v>0.95104895104895104</v>
       </c>
       <c r="C8" s="3">
-        <f>G8/$J8</f>
+        <f t="shared" si="1"/>
         <v>0.95104895104895104</v>
       </c>
       <c r="D8" s="3">
-        <f>H8/$J8</f>
+        <f t="shared" si="2"/>
         <v>1.0797202797202798</v>
       </c>
       <c r="E8" s="3">
-        <f>I8/$J8</f>
+        <f t="shared" si="3"/>
         <v>1.0181818181818181</v>
       </c>
       <c r="F8" s="1">
@@ -36848,7 +36874,7 @@
         <v>-1.8199999999999998E-8</v>
       </c>
       <c r="J8" s="1">
-        <f>AVERAGE(F8:I8)</f>
+        <f t="shared" si="4"/>
         <v>-1.7875E-8</v>
       </c>
     </row>
@@ -36857,19 +36883,19 @@
         <v>0.3</v>
       </c>
       <c r="B9" s="3">
-        <f>F9/$J9</f>
+        <f t="shared" si="0"/>
         <v>1.0777777777777777</v>
       </c>
       <c r="C9" s="3">
-        <f>G9/$J9</f>
+        <f t="shared" si="1"/>
         <v>0.91111111111111109</v>
       </c>
       <c r="D9" s="3">
-        <f>H9/$J9</f>
+        <f t="shared" si="2"/>
         <v>1.0777777777777777</v>
       </c>
       <c r="E9" s="3">
-        <f>I9/$J9</f>
+        <f t="shared" si="3"/>
         <v>0.93333333333333346</v>
       </c>
       <c r="F9" s="1">
@@ -36885,7 +36911,7 @@
         <v>-8.4000000000000024E-9</v>
       </c>
       <c r="J9" s="1">
-        <f>AVERAGE(F9:I9)</f>
+        <f t="shared" si="4"/>
         <v>-9.0000000000000012E-9</v>
       </c>
     </row>
@@ -36894,19 +36920,19 @@
         <v>0.35</v>
       </c>
       <c r="B10" s="3">
-        <f>F10/$J10</f>
+        <f t="shared" si="0"/>
         <v>1.0347741306467337</v>
       </c>
       <c r="C10" s="3">
-        <f>G10/$J10</f>
+        <f t="shared" si="1"/>
         <v>0.99577510562235949</v>
       </c>
       <c r="D10" s="3">
-        <f>H10/$J10</f>
+        <f t="shared" si="2"/>
         <v>0.96977575560610962</v>
       </c>
       <c r="E10" s="3">
-        <f>I10/$J10</f>
+        <f t="shared" si="3"/>
         <v>0.99967500812479682</v>
       </c>
       <c r="F10" s="1">
@@ -36922,7 +36948,7 @@
         <v>7.6900000000000007E-8</v>
       </c>
       <c r="J10" s="1">
-        <f>AVERAGE(F10:I10)</f>
+        <f t="shared" si="4"/>
         <v>7.6925000000000009E-8</v>
       </c>
     </row>
@@ -36931,19 +36957,19 @@
         <v>0.4</v>
       </c>
       <c r="B11" s="3">
-        <f>F11/$J11</f>
+        <f t="shared" si="0"/>
         <v>1.0251043066261225</v>
       </c>
       <c r="C11" s="3">
-        <f>G11/$J11</f>
+        <f t="shared" si="1"/>
         <v>0.99908068736298694</v>
       </c>
       <c r="D11" s="3">
-        <f>H11/$J11</f>
+        <f t="shared" si="2"/>
         <v>0.98027013648256833</v>
       </c>
       <c r="E11" s="3">
-        <f>I11/$J11</f>
+        <f t="shared" si="3"/>
         <v>0.99554486952832189</v>
       </c>
       <c r="F11" s="1">
@@ -36959,7 +36985,7 @@
         <v>7.0390000000000005E-7</v>
       </c>
       <c r="J11" s="1">
-        <f>AVERAGE(F11:I11)</f>
+        <f t="shared" si="4"/>
         <v>7.0705000000000007E-7</v>
       </c>
     </row>
@@ -36968,19 +36994,19 @@
         <v>0.45</v>
       </c>
       <c r="B12" s="3">
-        <f>F12/$J12</f>
+        <f t="shared" si="0"/>
         <v>1.0230792450513413</v>
       </c>
       <c r="C12" s="3">
-        <f>G12/$J12</f>
+        <f t="shared" si="1"/>
         <v>0.99843955448001354</v>
       </c>
       <c r="D12" s="3">
-        <f>H12/$J12</f>
+        <f t="shared" si="2"/>
         <v>0.98210859677576134</v>
       </c>
       <c r="E12" s="3">
-        <f>I12/$J12</f>
+        <f t="shared" si="3"/>
         <v>0.99637260369288383</v>
       </c>
       <c r="F12" s="1">
@@ -36996,7 +37022,7 @@
         <v>4.8686999999999997E-6</v>
       </c>
       <c r="J12" s="1">
-        <f>AVERAGE(F12:I12)</f>
+        <f t="shared" si="4"/>
         <v>4.8864249999999996E-6</v>
       </c>
     </row>
@@ -37005,19 +37031,19 @@
         <v>0.5</v>
       </c>
       <c r="B13" s="3">
-        <f>F13/$J13</f>
+        <f t="shared" si="0"/>
         <v>0.99987178033011637</v>
       </c>
       <c r="C13" s="3">
-        <f>G13/$J13</f>
+        <f t="shared" si="1"/>
         <v>1.0000246576288239</v>
       </c>
       <c r="D13" s="3">
-        <f>H13/$J13</f>
+        <f t="shared" si="2"/>
         <v>1.0000789044122362</v>
       </c>
       <c r="E13" s="3">
-        <f>I13/$J13</f>
+        <f t="shared" si="3"/>
         <v>1.0000246576288239</v>
       </c>
       <c r="F13" s="1">
@@ -37033,7 +37059,7 @@
         <v>2.0278199999999998E-5</v>
       </c>
       <c r="J13" s="1">
-        <f>AVERAGE(F13:I13)</f>
+        <f t="shared" si="4"/>
         <v>2.0277699999999997E-5</v>
       </c>
     </row>
@@ -37042,19 +37068,19 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="B14" s="3">
-        <f>F14/$J14</f>
+        <f t="shared" si="0"/>
         <v>1.0195401380489042</v>
       </c>
       <c r="C14" s="3">
-        <f>G14/$J14</f>
+        <f t="shared" si="1"/>
         <v>0.99782887355012184</v>
       </c>
       <c r="D14" s="3">
-        <f>H14/$J14</f>
+        <f t="shared" si="2"/>
         <v>0.98480211485085223</v>
       </c>
       <c r="E14" s="3">
-        <f>I14/$J14</f>
+        <f t="shared" si="3"/>
         <v>0.99782887355012184</v>
       </c>
       <c r="F14" s="1">
@@ -37070,7 +37096,7 @@
         <v>2.2979520000000002E-4</v>
       </c>
       <c r="J14" s="1">
-        <f>AVERAGE(F14:I14)</f>
+        <f t="shared" si="4"/>
         <v>2.302952E-4</v>
       </c>
     </row>
@@ -37079,19 +37105,19 @@
         <v>0.6</v>
       </c>
       <c r="B15" s="3">
-        <f>F15/$J15</f>
+        <f t="shared" si="0"/>
         <v>1.0163219390739602</v>
       </c>
       <c r="C15" s="3">
-        <f>G15/$J15</f>
+        <f t="shared" si="1"/>
         <v>0.99835310704804203</v>
       </c>
       <c r="D15" s="3">
-        <f>H15/$J15</f>
+        <f t="shared" si="2"/>
         <v>0.98757180783249088</v>
       </c>
       <c r="E15" s="3">
-        <f>I15/$J15</f>
+        <f t="shared" si="3"/>
         <v>0.99775314604550713</v>
       </c>
       <c r="F15" s="1">
@@ -37107,7 +37133,7 @@
         <v>1.66303E-3</v>
       </c>
       <c r="J15" s="1">
-        <f>AVERAGE(F15:I15)</f>
+        <f t="shared" si="4"/>
         <v>1.6667749999999999E-3</v>
       </c>
     </row>
@@ -37116,19 +37142,19 @@
         <v>0.65</v>
       </c>
       <c r="B16" s="3">
-        <f>F16/$J16</f>
+        <f t="shared" si="0"/>
         <v>1.0127337464012174</v>
       </c>
       <c r="C16" s="3">
-        <f>G16/$J16</f>
+        <f t="shared" si="1"/>
         <v>0.99735872702963635</v>
       </c>
       <c r="D16" s="3">
-        <f>H16/$J16</f>
+        <f t="shared" si="2"/>
         <v>0.9896678483732203</v>
       </c>
       <c r="E16" s="3">
-        <f>I16/$J16</f>
+        <f t="shared" si="3"/>
         <v>1.0002396781959257</v>
       </c>
       <c r="F16" s="1">
@@ -37144,7 +37170,7 @@
         <v>1.039142E-2</v>
       </c>
       <c r="J16" s="1">
-        <f>AVERAGE(F16:I16)</f>
+        <f t="shared" si="4"/>
         <v>1.0388930000000001E-2</v>
       </c>
     </row>
@@ -37153,19 +37179,19 @@
         <v>0.7</v>
       </c>
       <c r="B17" s="3">
-        <f>F17/$J17</f>
+        <f t="shared" si="0"/>
         <v>1.0000110795003392</v>
       </c>
       <c r="C17" s="3">
-        <f>G17/$J17</f>
+        <f t="shared" si="1"/>
         <v>1.0000012310555932</v>
       </c>
       <c r="D17" s="3">
-        <f>H17/$J17</f>
+        <f t="shared" si="2"/>
         <v>0.9999913826108473</v>
       </c>
       <c r="E17" s="3">
-        <f>I17/$J17</f>
+        <f t="shared" si="3"/>
         <v>0.99999630683322016</v>
       </c>
       <c r="F17" s="1">
@@ -37181,7 +37207,7 @@
         <v>2.0307699999999998E-2</v>
       </c>
       <c r="J17" s="1">
-        <f>AVERAGE(F17:I17)</f>
+        <f t="shared" si="4"/>
         <v>2.0307775E-2</v>
       </c>
     </row>
@@ -37190,19 +37216,19 @@
         <v>0.75</v>
       </c>
       <c r="B18" s="3">
-        <f>F18/$J18</f>
+        <f t="shared" si="0"/>
         <v>1.0000123106923287</v>
       </c>
       <c r="C18" s="3">
-        <f>G18/$J18</f>
+        <f t="shared" si="1"/>
         <v>1.0000024621384656</v>
       </c>
       <c r="D18" s="3">
-        <f>H18/$J18</f>
+        <f t="shared" si="2"/>
         <v>0.99999261358460267</v>
       </c>
       <c r="E18" s="3">
-        <f>I18/$J18</f>
+        <f t="shared" si="3"/>
         <v>0.99999261358460267</v>
       </c>
       <c r="F18" s="1">
@@ -37218,7 +37244,7 @@
         <v>2.03074E-2</v>
       </c>
       <c r="J18" s="1">
-        <f>AVERAGE(F18:I18)</f>
+        <f t="shared" si="4"/>
         <v>2.0307550000000001E-2</v>
       </c>
     </row>
@@ -37227,19 +37253,19 @@
         <v>0.8</v>
       </c>
       <c r="B19" s="3">
-        <f>F19/$J19</f>
+        <f t="shared" si="0"/>
         <v>1.0000123108135723</v>
       </c>
       <c r="C19" s="3">
-        <f>G19/$J19</f>
+        <f t="shared" si="1"/>
         <v>1.0000024621627146</v>
       </c>
       <c r="D19" s="3">
-        <f>H19/$J19</f>
+        <f t="shared" si="2"/>
         <v>0.99999261351185664</v>
       </c>
       <c r="E19" s="3">
-        <f>I19/$J19</f>
+        <f t="shared" si="3"/>
         <v>0.99999261351185664</v>
       </c>
       <c r="F19" s="1">
@@ -37255,7 +37281,7 @@
         <v>2.0307200000000001E-2</v>
       </c>
       <c r="J19" s="1">
-        <f>AVERAGE(F19:I19)</f>
+        <f t="shared" si="4"/>
         <v>2.0307349999999998E-2</v>
       </c>
     </row>
@@ -37264,19 +37290,19 @@
         <v>0.85</v>
       </c>
       <c r="B20" s="3">
-        <f>F20/$J20</f>
+        <f t="shared" si="0"/>
         <v>1.0000123109954424</v>
       </c>
       <c r="C20" s="3">
-        <f>G20/$J20</f>
+        <f t="shared" si="1"/>
         <v>1.0000024621990884</v>
       </c>
       <c r="D20" s="3">
-        <f>H20/$J20</f>
+        <f t="shared" si="2"/>
         <v>0.99999261340273449</v>
       </c>
       <c r="E20" s="3">
-        <f>I20/$J20</f>
+        <f t="shared" si="3"/>
         <v>0.99999261340273449</v>
       </c>
       <c r="F20" s="1">
@@ -37292,7 +37318,7 @@
         <v>2.0306899999999999E-2</v>
       </c>
       <c r="J20" s="1">
-        <f>AVERAGE(F20:I20)</f>
+        <f t="shared" si="4"/>
         <v>2.030705E-2</v>
       </c>
     </row>
@@ -37301,19 +37327,19 @@
         <v>0.9</v>
       </c>
       <c r="B21" s="3">
-        <f>F21/$J21</f>
+        <f t="shared" si="0"/>
         <v>1.0000110800459452</v>
       </c>
       <c r="C21" s="3">
-        <f>G21/$J21</f>
+        <f t="shared" si="1"/>
         <v>1.0000012311162161</v>
       </c>
       <c r="D21" s="3">
-        <f>H21/$J21</f>
+        <f t="shared" si="2"/>
         <v>0.99999138218648709</v>
       </c>
       <c r="E21" s="3">
-        <f>I21/$J21</f>
+        <f t="shared" si="3"/>
         <v>0.99999630665135164</v>
       </c>
       <c r="F21" s="1">
@@ -37329,7 +37355,7 @@
         <v>2.03067E-2</v>
       </c>
       <c r="J21" s="1">
-        <f>AVERAGE(F21:I21)</f>
+        <f t="shared" si="4"/>
         <v>2.0306774999999999E-2</v>
       </c>
     </row>
@@ -37338,19 +37364,19 @@
         <v>0.95</v>
       </c>
       <c r="B22" s="3">
-        <f>F22/$J22</f>
+        <f t="shared" si="0"/>
         <v>1.0000135424451009</v>
       </c>
       <c r="C22" s="3">
-        <f>G22/$J22</f>
+        <f t="shared" si="1"/>
         <v>1.0000036933941185</v>
       </c>
       <c r="D22" s="3">
-        <f>H22/$J22</f>
+        <f t="shared" si="2"/>
         <v>0.99998891981764482</v>
       </c>
       <c r="E22" s="3">
-        <f>I22/$J22</f>
+        <f t="shared" si="3"/>
         <v>0.99999384434313598</v>
       </c>
       <c r="F22" s="1">
@@ -37366,7 +37392,7 @@
         <v>2.0306399999999999E-2</v>
       </c>
       <c r="J22" s="1">
-        <f>AVERAGE(F22:I22)</f>
+        <f t="shared" si="4"/>
         <v>2.0306524999999999E-2</v>
       </c>
     </row>
@@ -37375,19 +37401,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="3">
-        <f>F23/$J23</f>
+        <f t="shared" si="0"/>
         <v>1.0000123114804556</v>
       </c>
       <c r="C23" s="3">
-        <f>G23/$J23</f>
+        <f t="shared" si="1"/>
         <v>1.0000024622960912</v>
       </c>
       <c r="D23" s="3">
-        <f>H23/$J23</f>
+        <f t="shared" si="2"/>
         <v>0.99999261311172682</v>
       </c>
       <c r="E23" s="3">
-        <f>I23/$J23</f>
+        <f t="shared" si="3"/>
         <v>0.99999261311172682</v>
       </c>
       <c r="F23" s="1">
@@ -37403,7 +37429,7 @@
         <v>2.0306100000000001E-2</v>
       </c>
       <c r="J23" s="1">
-        <f>AVERAGE(F23:I23)</f>
+        <f t="shared" si="4"/>
         <v>2.0306249999999998E-2</v>
       </c>
     </row>
@@ -37412,19 +37438,19 @@
         <v>1.05</v>
       </c>
       <c r="B24" s="3">
-        <f>F24/$J24</f>
+        <f t="shared" si="0"/>
         <v>1.0000123116623454</v>
       </c>
       <c r="C24" s="3">
-        <f>G24/$J24</f>
+        <f t="shared" si="1"/>
         <v>1.000002462332469</v>
       </c>
       <c r="D24" s="3">
-        <f>H24/$J24</f>
+        <f t="shared" si="2"/>
         <v>0.99999261300259279</v>
       </c>
       <c r="E24" s="3">
-        <f>I24/$J24</f>
+        <f t="shared" si="3"/>
         <v>0.99999261300259279</v>
       </c>
       <c r="F24" s="1">
@@ -37440,7 +37466,7 @@
         <v>2.0305799999999999E-2</v>
       </c>
       <c r="J24" s="1">
-        <f>AVERAGE(F24:I24)</f>
+        <f t="shared" si="4"/>
         <v>2.030595E-2</v>
       </c>
     </row>
@@ -37449,19 +37475,19 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B25" s="3">
-        <f>F25/$J25</f>
+        <f t="shared" si="0"/>
         <v>1.0000123118442403</v>
       </c>
       <c r="C25" s="3">
-        <f>G25/$J25</f>
+        <f t="shared" si="1"/>
         <v>1.0000024623688479</v>
       </c>
       <c r="D25" s="3">
-        <f>H25/$J25</f>
+        <f t="shared" si="2"/>
         <v>0.99999261289345576</v>
       </c>
       <c r="E25" s="3">
-        <f>I25/$J25</f>
+        <f t="shared" si="3"/>
         <v>0.99999261289345576</v>
       </c>
       <c r="F25" s="1">
@@ -37477,7 +37503,7 @@
         <v>2.0305500000000001E-2</v>
       </c>
       <c r="J25" s="1">
-        <f>AVERAGE(F25:I25)</f>
+        <f t="shared" si="4"/>
         <v>2.0305650000000001E-2</v>
       </c>
     </row>
@@ -37486,19 +37512,19 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="B26" s="3">
-        <f>F26/$J26</f>
+        <f t="shared" si="0"/>
         <v>1.0000123120261408</v>
       </c>
       <c r="C26" s="3">
-        <f>G26/$J26</f>
+        <f t="shared" si="1"/>
         <v>1.0000024624052282</v>
       </c>
       <c r="D26" s="3">
-        <f>H26/$J26</f>
+        <f t="shared" si="2"/>
         <v>0.99999261278431539</v>
       </c>
       <c r="E26" s="3">
-        <f>I26/$J26</f>
+        <f t="shared" si="3"/>
         <v>0.99999261278431539</v>
       </c>
       <c r="F26" s="1">
@@ -37514,7 +37540,7 @@
         <v>2.0305199999999999E-2</v>
       </c>
       <c r="J26" s="1">
-        <f>AVERAGE(F26:I26)</f>
+        <f t="shared" si="4"/>
         <v>2.030535E-2</v>
       </c>
     </row>
@@ -37523,19 +37549,19 @@
         <v>1.2</v>
       </c>
       <c r="B27" s="3">
-        <f>F27/$J27</f>
+        <f t="shared" si="0"/>
         <v>1.0000123122080469</v>
       </c>
       <c r="C27" s="3">
-        <f>G27/$J27</f>
+        <f t="shared" si="1"/>
         <v>1.0000024624416095</v>
       </c>
       <c r="D27" s="3">
-        <f>H27/$J27</f>
+        <f t="shared" si="2"/>
         <v>0.99999261267517203</v>
       </c>
       <c r="E27" s="3">
-        <f>I27/$J27</f>
+        <f t="shared" si="3"/>
         <v>0.99999261267517203</v>
       </c>
       <c r="F27" s="1">
@@ -37551,7 +37577,7 @@
         <v>2.0304900000000001E-2</v>
       </c>
       <c r="J27" s="1">
-        <f>AVERAGE(F27:I27)</f>
+        <f t="shared" si="4"/>
         <v>2.0305049999999998E-2</v>
       </c>
     </row>
@@ -37560,19 +37586,19 @@
         <v>1.25</v>
       </c>
       <c r="B28" s="3">
-        <f>F28/$J28</f>
+        <f t="shared" si="0"/>
         <v>1.000012312389958</v>
       </c>
       <c r="C28" s="3">
-        <f>G28/$J28</f>
+        <f t="shared" si="1"/>
         <v>1.0000024624779917</v>
       </c>
       <c r="D28" s="3">
-        <f>H28/$J28</f>
+        <f t="shared" si="2"/>
         <v>0.99999261256602512</v>
       </c>
       <c r="E28" s="3">
-        <f>I28/$J28</f>
+        <f t="shared" si="3"/>
         <v>0.99999261256602512</v>
       </c>
       <c r="F28" s="1">
@@ -37588,7 +37614,7 @@
         <v>2.0304599999999999E-2</v>
       </c>
       <c r="J28" s="1">
-        <f>AVERAGE(F28:I28)</f>
+        <f t="shared" si="4"/>
         <v>2.030475E-2</v>
       </c>
     </row>
@@ -37597,19 +37623,19 @@
         <v>1.3</v>
       </c>
       <c r="B29" s="3">
-        <f>F29/$J29</f>
+        <f t="shared" si="0"/>
         <v>1.0000123125718747</v>
       </c>
       <c r="C29" s="3">
-        <f>G29/$J29</f>
+        <f t="shared" si="1"/>
         <v>1.0000024625143751</v>
       </c>
       <c r="D29" s="3">
-        <f>H29/$J29</f>
+        <f t="shared" si="2"/>
         <v>0.99999261245687532</v>
       </c>
       <c r="E29" s="3">
-        <f>I29/$J29</f>
+        <f t="shared" si="3"/>
         <v>0.99999261245687532</v>
       </c>
       <c r="F29" s="1">
@@ -37625,7 +37651,7 @@
         <v>2.0304300000000001E-2</v>
       </c>
       <c r="J29" s="1">
-        <f>AVERAGE(F29:I29)</f>
+        <f t="shared" si="4"/>
         <v>2.0304449999999998E-2</v>
       </c>
     </row>
@@ -37634,19 +37660,19 @@
         <v>1.35</v>
       </c>
       <c r="B30" s="3">
-        <f>F30/$J30</f>
+        <f t="shared" si="0"/>
         <v>1.0000123127537965</v>
       </c>
       <c r="C30" s="3">
-        <f>G30/$J30</f>
+        <f t="shared" si="1"/>
         <v>1.0000024625507593</v>
       </c>
       <c r="D30" s="3">
-        <f>H30/$J30</f>
+        <f t="shared" si="2"/>
         <v>0.99999261234772197</v>
       </c>
       <c r="E30" s="3">
-        <f>I30/$J30</f>
+        <f t="shared" si="3"/>
         <v>0.99999261234772197</v>
       </c>
       <c r="F30" s="1">
@@ -37662,7 +37688,7 @@
         <v>2.0303999999999999E-2</v>
       </c>
       <c r="J30" s="1">
-        <f>AVERAGE(F30:I30)</f>
+        <f t="shared" si="4"/>
         <v>2.030415E-2</v>
       </c>
     </row>
@@ -37671,19 +37697,19 @@
         <v>1.4</v>
       </c>
       <c r="B31" s="3">
-        <f>F31/$J31</f>
+        <f t="shared" si="0"/>
         <v>1.0000098503728365</v>
       </c>
       <c r="C31" s="3">
-        <f>G31/$J31</f>
+        <f t="shared" si="1"/>
         <v>1.0000049251864183</v>
       </c>
       <c r="D31" s="3">
-        <f>H31/$J31</f>
+        <f t="shared" si="2"/>
         <v>0.99999014962716326</v>
       </c>
       <c r="E31" s="3">
-        <f>I31/$J31</f>
+        <f t="shared" si="3"/>
         <v>0.99999507481358174</v>
       </c>
       <c r="F31" s="1">
@@ -37699,7 +37725,7 @@
         <v>2.0303700000000001E-2</v>
       </c>
       <c r="J31" s="1">
-        <f>AVERAGE(F31:I31)</f>
+        <f t="shared" si="4"/>
         <v>2.03038E-2</v>
       </c>
     </row>
@@ -37708,19 +37734,19 @@
         <v>1.45</v>
       </c>
       <c r="B32" s="3">
-        <f>F32/$J32</f>
+        <f t="shared" si="0"/>
         <v>1.0000110818468269</v>
       </c>
       <c r="C32" s="3">
-        <f>G32/$J32</f>
+        <f t="shared" si="1"/>
         <v>1.000001231316314</v>
       </c>
       <c r="D32" s="3">
-        <f>H32/$J32</f>
+        <f t="shared" si="2"/>
         <v>0.99999138078580152</v>
       </c>
       <c r="E32" s="3">
-        <f>I32/$J32</f>
+        <f t="shared" si="3"/>
         <v>0.99999630605105783</v>
       </c>
       <c r="F32" s="1">
@@ -37736,7 +37762,7 @@
         <v>2.0303399999999999E-2</v>
       </c>
       <c r="J32" s="1">
-        <f>AVERAGE(F32:I32)</f>
+        <f t="shared" si="4"/>
         <v>2.0303474999999998E-2</v>
       </c>
     </row>
@@ -37745,19 +37771,19 @@
         <v>1.5</v>
       </c>
       <c r="B33" s="3">
-        <f>F33/$J33</f>
+        <f t="shared" si="0"/>
         <v>1.0000123133602421</v>
       </c>
       <c r="C33" s="3">
-        <f>G33/$J33</f>
+        <f t="shared" si="1"/>
         <v>1.0000024626720485</v>
       </c>
       <c r="D33" s="3">
-        <f>H33/$J33</f>
+        <f t="shared" si="2"/>
         <v>0.9999926119838547</v>
       </c>
       <c r="E33" s="3">
-        <f>I33/$J33</f>
+        <f t="shared" si="3"/>
         <v>0.9999926119838547</v>
       </c>
       <c r="F33" s="1">
@@ -37773,7 +37799,7 @@
         <v>2.0302999999999998E-2</v>
       </c>
       <c r="J33" s="1">
-        <f>AVERAGE(F33:I33)</f>
+        <f t="shared" si="4"/>
         <v>2.0303149999999999E-2</v>
       </c>
     </row>
@@ -37782,19 +37808,19 @@
         <v>1.55</v>
       </c>
       <c r="B34" s="3">
-        <f>F34/$J34</f>
+        <f t="shared" si="0"/>
         <v>1.0000123135421874</v>
       </c>
       <c r="C34" s="3">
-        <f>G34/$J34</f>
+        <f t="shared" si="1"/>
         <v>1.0000024627084374</v>
       </c>
       <c r="D34" s="3">
-        <f>H34/$J34</f>
+        <f t="shared" si="2"/>
         <v>0.99999261187468746</v>
       </c>
       <c r="E34" s="3">
-        <f>I34/$J34</f>
+        <f t="shared" si="3"/>
         <v>0.99999261187468746</v>
       </c>
       <c r="F34" s="1">
@@ -37810,7 +37836,7 @@
         <v>2.03027E-2</v>
       </c>
       <c r="J34" s="1">
-        <f>AVERAGE(F34:I34)</f>
+        <f t="shared" si="4"/>
         <v>2.0302850000000001E-2</v>
       </c>
     </row>
@@ -37819,19 +37845,19 @@
         <v>1.6</v>
       </c>
       <c r="B35" s="3">
-        <f>F35/$J35</f>
+        <f t="shared" ref="B35:B66" si="5">F35/$J35</f>
         <v>1.0000123137241381</v>
       </c>
       <c r="C35" s="3">
-        <f>G35/$J35</f>
+        <f t="shared" ref="C35:C66" si="6">G35/$J35</f>
         <v>1.0000024627448276</v>
       </c>
       <c r="D35" s="3">
-        <f>H35/$J35</f>
+        <f t="shared" ref="D35:D66" si="7">H35/$J35</f>
         <v>0.99999261176551713</v>
       </c>
       <c r="E35" s="3">
-        <f>I35/$J35</f>
+        <f t="shared" ref="E35:E66" si="8">I35/$J35</f>
         <v>0.99999261176551713</v>
       </c>
       <c r="F35" s="1">
@@ -37847,7 +37873,7 @@
         <v>2.0302399999999998E-2</v>
       </c>
       <c r="J35" s="1">
-        <f>AVERAGE(F35:I35)</f>
+        <f t="shared" ref="J35:J66" si="9">AVERAGE(F35:I35)</f>
         <v>2.0302549999999999E-2</v>
       </c>
     </row>
@@ -37856,19 +37882,19 @@
         <v>1.65</v>
       </c>
       <c r="B36" s="3">
-        <f>F36/$J36</f>
+        <f t="shared" si="5"/>
         <v>1.0000098511491364</v>
       </c>
       <c r="C36" s="3">
-        <f>G36/$J36</f>
+        <f t="shared" si="6"/>
         <v>1.0000049255745682</v>
       </c>
       <c r="D36" s="3">
-        <f>H36/$J36</f>
+        <f t="shared" si="7"/>
         <v>0.99999014885086346</v>
       </c>
       <c r="E36" s="3">
-        <f>I36/$J36</f>
+        <f t="shared" si="8"/>
         <v>0.99999507442543178</v>
       </c>
       <c r="F36" s="1">
@@ -37884,7 +37910,7 @@
         <v>2.03021E-2</v>
       </c>
       <c r="J36" s="1">
-        <f>AVERAGE(F36:I36)</f>
+        <f t="shared" si="9"/>
         <v>2.0302199999999999E-2</v>
       </c>
     </row>
@@ -37893,19 +37919,19 @@
         <v>1.7</v>
       </c>
       <c r="B37" s="3">
-        <f>F37/$J37</f>
+        <f t="shared" si="5"/>
         <v>1.000011082720192</v>
       </c>
       <c r="C37" s="3">
-        <f>G37/$J37</f>
+        <f t="shared" si="6"/>
         <v>1.0000012314133546</v>
       </c>
       <c r="D37" s="3">
-        <f>H37/$J37</f>
+        <f t="shared" si="7"/>
         <v>0.99999138010651722</v>
       </c>
       <c r="E37" s="3">
-        <f>I37/$J37</f>
+        <f t="shared" si="8"/>
         <v>0.99999630575993581</v>
       </c>
       <c r="F37" s="1">
@@ -37921,7 +37947,7 @@
         <v>2.0301799999999998E-2</v>
       </c>
       <c r="J37" s="1">
-        <f>AVERAGE(F37:I37)</f>
+        <f t="shared" si="9"/>
         <v>2.0301875E-2</v>
       </c>
     </row>
@@ -37930,19 +37956,19 @@
         <v>1.75</v>
       </c>
       <c r="B38" s="3">
-        <f>F38/$J38</f>
+        <f t="shared" si="5"/>
         <v>1.0000110828839635</v>
       </c>
       <c r="C38" s="3">
-        <f>G38/$J38</f>
+        <f t="shared" si="6"/>
         <v>1.0000012314315516</v>
       </c>
       <c r="D38" s="3">
-        <f>H38/$J38</f>
+        <f t="shared" si="7"/>
         <v>0.99999137997913967</v>
       </c>
       <c r="E38" s="3">
-        <f>I38/$J38</f>
+        <f t="shared" si="8"/>
         <v>0.99999630570534559</v>
       </c>
       <c r="F38" s="1">
@@ -37958,7 +37984,7 @@
         <v>2.03015E-2</v>
       </c>
       <c r="J38" s="1">
-        <f>AVERAGE(F38:I38)</f>
+        <f t="shared" si="9"/>
         <v>2.0301574999999999E-2</v>
       </c>
     </row>
@@ -37967,19 +37993,19 @@
         <v>1.8</v>
       </c>
       <c r="B39" s="3">
-        <f>F39/$J39</f>
+        <f t="shared" si="5"/>
         <v>1.0000123145126532</v>
       </c>
       <c r="C39" s="3">
-        <f>G39/$J39</f>
+        <f t="shared" si="6"/>
         <v>1.0000024629025308</v>
       </c>
       <c r="D39" s="3">
-        <f>H39/$J39</f>
+        <f t="shared" si="7"/>
         <v>0.99999261129240802</v>
       </c>
       <c r="E39" s="3">
-        <f>I39/$J39</f>
+        <f t="shared" si="8"/>
         <v>0.99999261129240802</v>
       </c>
       <c r="F39" s="1">
@@ -37995,7 +38021,7 @@
         <v>2.0301099999999999E-2</v>
       </c>
       <c r="J39" s="1">
-        <f>AVERAGE(F39:I39)</f>
+        <f t="shared" si="9"/>
         <v>2.030125E-2</v>
       </c>
     </row>
@@ -38004,19 +38030,19 @@
         <v>1.85</v>
       </c>
       <c r="B40" s="3">
-        <f>F40/$J40</f>
+        <f t="shared" si="5"/>
         <v>1.0000123146946325</v>
       </c>
       <c r="C40" s="3">
-        <f>G40/$J40</f>
+        <f t="shared" si="6"/>
         <v>1.0000024629389266</v>
       </c>
       <c r="D40" s="3">
-        <f>H40/$J40</f>
+        <f t="shared" si="7"/>
         <v>0.99999261118322058</v>
       </c>
       <c r="E40" s="3">
-        <f>I40/$J40</f>
+        <f t="shared" si="8"/>
         <v>0.99999261118322058</v>
       </c>
       <c r="F40" s="1">
@@ -38032,7 +38058,7 @@
         <v>2.0300800000000001E-2</v>
       </c>
       <c r="J40" s="1">
-        <f>AVERAGE(F40:I40)</f>
+        <f t="shared" si="9"/>
         <v>2.0300949999999998E-2</v>
       </c>
     </row>
@@ -38041,19 +38067,19 @@
         <v>1.9</v>
       </c>
       <c r="B41" s="3">
-        <f>F41/$J41</f>
+        <f t="shared" si="5"/>
         <v>1.0000123148766173</v>
       </c>
       <c r="C41" s="3">
-        <f>G41/$J41</f>
+        <f t="shared" si="6"/>
         <v>1.0000024629753232</v>
       </c>
       <c r="D41" s="3">
-        <f>H41/$J41</f>
+        <f t="shared" si="7"/>
         <v>0.99999261107402959</v>
       </c>
       <c r="E41" s="3">
-        <f>I41/$J41</f>
+        <f t="shared" si="8"/>
         <v>0.99999261107402959</v>
       </c>
       <c r="F41" s="1">
@@ -38069,7 +38095,7 @@
         <v>2.0300499999999999E-2</v>
       </c>
       <c r="J41" s="1">
-        <f>AVERAGE(F41:I41)</f>
+        <f t="shared" si="9"/>
         <v>2.030065E-2</v>
       </c>
     </row>
@@ -38078,19 +38104,19 @@
         <v>1.95</v>
       </c>
       <c r="B42" s="3">
-        <f>F42/$J42</f>
+        <f t="shared" si="5"/>
         <v>1.0000086205516414</v>
       </c>
       <c r="C42" s="3">
-        <f>G42/$J42</f>
+        <f t="shared" si="6"/>
         <v>1.000003694522132</v>
       </c>
       <c r="D42" s="3">
-        <f>H42/$J42</f>
+        <f t="shared" si="7"/>
         <v>0.99999384246311329</v>
       </c>
       <c r="E42" s="3">
-        <f>I42/$J42</f>
+        <f t="shared" si="8"/>
         <v>0.99999384246311329</v>
       </c>
       <c r="F42" s="1">
@@ -38106,7 +38132,7 @@
         <v>2.0300200000000001E-2</v>
       </c>
       <c r="J42" s="1">
-        <f>AVERAGE(F42:I42)</f>
+        <f t="shared" si="9"/>
         <v>2.0300325000000001E-2</v>
       </c>
     </row>
@@ -38115,19 +38141,19 @@
         <v>2</v>
       </c>
       <c r="B43" s="3">
-        <f>F43/$J43</f>
+        <f t="shared" si="5"/>
         <v>1.0000098522167489</v>
       </c>
       <c r="C43" s="3">
-        <f>G43/$J43</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="D43" s="3">
-        <f>H43/$J43</f>
+        <f t="shared" si="7"/>
         <v>0.99999507389162567</v>
       </c>
       <c r="E43" s="3">
-        <f>I43/$J43</f>
+        <f t="shared" si="8"/>
         <v>0.99999507389162567</v>
       </c>
       <c r="F43" s="1">
@@ -38143,7 +38169,7 @@
         <v>2.0299899999999999E-2</v>
       </c>
       <c r="J43" s="1">
-        <f>AVERAGE(F43:I43)</f>
+        <f t="shared" si="9"/>
         <v>2.0299999999999999E-2</v>
       </c>
     </row>
@@ -38152,19 +38178,19 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="B44" s="3">
-        <f>F44/$J44</f>
+        <f t="shared" si="5"/>
         <v>1.0000098523623502</v>
       </c>
       <c r="C44" s="3">
-        <f>G44/$J44</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="D44" s="3">
-        <f>H44/$J44</f>
+        <f t="shared" si="7"/>
         <v>0.99999507381882491</v>
       </c>
       <c r="E44" s="3">
-        <f>I44/$J44</f>
+        <f t="shared" si="8"/>
         <v>0.99999507381882491</v>
       </c>
       <c r="F44" s="1">
@@ -38180,7 +38206,7 @@
         <v>2.0299600000000001E-2</v>
       </c>
       <c r="J44" s="1">
-        <f>AVERAGE(F44:I44)</f>
+        <f t="shared" si="9"/>
         <v>2.02997E-2</v>
       </c>
     </row>
@@ -38189,19 +38215,19 @@
         <v>2.1</v>
       </c>
       <c r="B45" s="3">
-        <f>F45/$J45</f>
+        <f t="shared" si="5"/>
         <v>1.00001231566528</v>
       </c>
       <c r="C45" s="3">
-        <f>G45/$J45</f>
+        <f t="shared" si="6"/>
         <v>1.000002463133056</v>
       </c>
       <c r="D45" s="3">
-        <f>H45/$J45</f>
+        <f t="shared" si="7"/>
         <v>0.999992610600832</v>
       </c>
       <c r="E45" s="3">
-        <f>I45/$J45</f>
+        <f t="shared" si="8"/>
         <v>0.999992610600832</v>
       </c>
       <c r="F45" s="1">
@@ -38217,7 +38243,7 @@
         <v>2.02992E-2</v>
       </c>
       <c r="J45" s="1">
-        <f>AVERAGE(F45:I45)</f>
+        <f t="shared" si="9"/>
         <v>2.0299350000000001E-2</v>
       </c>
     </row>
@@ -38226,19 +38252,19 @@
         <v>2.15</v>
       </c>
       <c r="B46" s="3">
-        <f>F46/$J46</f>
+        <f t="shared" si="5"/>
         <v>1.0000123158472933</v>
       </c>
       <c r="C46" s="3">
-        <f>G46/$J46</f>
+        <f t="shared" si="6"/>
         <v>1.0000024631694588</v>
       </c>
       <c r="D46" s="3">
-        <f>H46/$J46</f>
+        <f t="shared" si="7"/>
         <v>0.99999261049162391</v>
       </c>
       <c r="E46" s="3">
-        <f>I46/$J46</f>
+        <f t="shared" si="8"/>
         <v>0.99999261049162391</v>
       </c>
       <c r="F46" s="1">
@@ -38254,7 +38280,7 @@
         <v>2.0298899999999998E-2</v>
       </c>
       <c r="J46" s="1">
-        <f>AVERAGE(F46:I46)</f>
+        <f t="shared" si="9"/>
         <v>2.0299049999999999E-2</v>
       </c>
     </row>
@@ -38263,19 +38289,19 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B47" s="3">
-        <f>F47/$J47</f>
+        <f t="shared" si="5"/>
         <v>1.0000098528477193</v>
       </c>
       <c r="C47" s="3">
-        <f>G47/$J47</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="D47" s="3">
-        <f>H47/$J47</f>
+        <f t="shared" si="7"/>
         <v>0.99999507357614037</v>
       </c>
       <c r="E47" s="3">
-        <f>I47/$J47</f>
+        <f t="shared" si="8"/>
         <v>0.99999507357614037</v>
       </c>
       <c r="F47" s="1">
@@ -38291,7 +38317,7 @@
         <v>2.02986E-2</v>
       </c>
       <c r="J47" s="1">
-        <f>AVERAGE(F47:I47)</f>
+        <f t="shared" si="9"/>
         <v>2.0298699999999999E-2</v>
       </c>
     </row>
@@ -38300,19 +38326,19 @@
         <v>2.25</v>
       </c>
       <c r="B48" s="3">
-        <f>F48/$J48</f>
+        <f t="shared" si="5"/>
         <v>1.000011084631159</v>
       </c>
       <c r="C48" s="3">
-        <f>G48/$J48</f>
+        <f t="shared" si="6"/>
         <v>1.0000012316256843</v>
       </c>
       <c r="D48" s="3">
-        <f>H48/$J48</f>
+        <f t="shared" si="7"/>
         <v>0.9999913786202097</v>
       </c>
       <c r="E48" s="3">
-        <f>I48/$J48</f>
+        <f t="shared" si="8"/>
         <v>0.9999963051229469</v>
       </c>
       <c r="F48" s="1">
@@ -38328,7 +38354,7 @@
         <v>2.0298299999999998E-2</v>
       </c>
       <c r="J48" s="1">
-        <f>AVERAGE(F48:I48)</f>
+        <f t="shared" si="9"/>
         <v>2.0298375E-2</v>
       </c>
     </row>
@@ -38337,19 +38363,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B49" s="3">
-        <f>F49/$J49</f>
+        <f t="shared" si="5"/>
         <v>1.0000123164540435</v>
       </c>
       <c r="C49" s="3">
-        <f>G49/$J49</f>
+        <f t="shared" si="6"/>
         <v>1.0000024632908089</v>
       </c>
       <c r="D49" s="3">
-        <f>H49/$J49</f>
+        <f t="shared" si="7"/>
         <v>0.99999261012757401</v>
       </c>
       <c r="E49" s="3">
-        <f>I49/$J49</f>
+        <f t="shared" si="8"/>
         <v>0.99999261012757401</v>
       </c>
       <c r="F49" s="1">
@@ -38365,7 +38391,7 @@
         <v>2.0297900000000001E-2</v>
       </c>
       <c r="J49" s="1">
-        <f>AVERAGE(F49:I49)</f>
+        <f t="shared" si="9"/>
         <v>2.0298049999999998E-2</v>
       </c>
     </row>
@@ -38374,19 +38400,19 @@
         <v>2.35</v>
       </c>
       <c r="B50" s="3">
-        <f>F50/$J50</f>
+        <f t="shared" si="5"/>
         <v>1.0000086216558752</v>
       </c>
       <c r="C50" s="3">
-        <f>G50/$J50</f>
+        <f t="shared" si="6"/>
         <v>1.0000036949953752</v>
       </c>
       <c r="D50" s="3">
-        <f>H50/$J50</f>
+        <f t="shared" si="7"/>
         <v>0.99999384167437488</v>
       </c>
       <c r="E50" s="3">
-        <f>I50/$J50</f>
+        <f t="shared" si="8"/>
         <v>0.99999384167437488</v>
       </c>
       <c r="F50" s="1">
@@ -38402,7 +38428,7 @@
         <v>2.0297599999999999E-2</v>
       </c>
       <c r="J50" s="1">
-        <f>AVERAGE(F50:I50)</f>
+        <f t="shared" si="9"/>
         <v>2.0297724999999999E-2</v>
       </c>
     </row>
@@ -38411,19 +38437,19 @@
         <v>2.4</v>
       </c>
       <c r="B51" s="3">
-        <f>F51/$J51</f>
+        <f t="shared" si="5"/>
         <v>1.0000110851772703</v>
       </c>
       <c r="C51" s="3">
-        <f>G51/$J51</f>
+        <f t="shared" si="6"/>
         <v>1.0000012316863633</v>
       </c>
       <c r="D51" s="3">
-        <f>H51/$J51</f>
+        <f t="shared" si="7"/>
         <v>0.99999137819545636</v>
       </c>
       <c r="E51" s="3">
-        <f>I51/$J51</f>
+        <f t="shared" si="8"/>
         <v>0.99999630494090996</v>
       </c>
       <c r="F51" s="1">
@@ -38439,7 +38465,7 @@
         <v>2.0297300000000001E-2</v>
       </c>
       <c r="J51" s="1">
-        <f>AVERAGE(F51:I51)</f>
+        <f t="shared" si="9"/>
         <v>2.0297374999999999E-2</v>
       </c>
     </row>
@@ -38448,19 +38474,19 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="B52" s="3">
-        <f>F52/$J52</f>
+        <f t="shared" si="5"/>
         <v>1.0000123170608537</v>
       </c>
       <c r="C52" s="3">
-        <f>G52/$J52</f>
+        <f t="shared" si="6"/>
         <v>1.0000024634121707</v>
       </c>
       <c r="D52" s="3">
-        <f>H52/$J52</f>
+        <f t="shared" si="7"/>
         <v>0.99999260976348781</v>
       </c>
       <c r="E52" s="3">
-        <f>I52/$J52</f>
+        <f t="shared" si="8"/>
         <v>0.99999260976348781</v>
       </c>
       <c r="F52" s="1">
@@ -38476,7 +38502,7 @@
         <v>2.02969E-2</v>
       </c>
       <c r="J52" s="1">
-        <f>AVERAGE(F52:I52)</f>
+        <f t="shared" si="9"/>
         <v>2.0297050000000001E-2</v>
       </c>
     </row>
@@ -38485,19 +38511,19 @@
         <v>2.5</v>
       </c>
       <c r="B53" s="3">
-        <f>F53/$J53</f>
+        <f t="shared" si="5"/>
         <v>1.0000123172429083</v>
       </c>
       <c r="C53" s="3">
-        <f>G53/$J53</f>
+        <f t="shared" si="6"/>
         <v>1.0000024634485818</v>
       </c>
       <c r="D53" s="3">
-        <f>H53/$J53</f>
+        <f t="shared" si="7"/>
         <v>0.99999260965425496</v>
       </c>
       <c r="E53" s="3">
-        <f>I53/$J53</f>
+        <f t="shared" si="8"/>
         <v>0.99999260965425496</v>
       </c>
       <c r="F53" s="1">
@@ -38513,7 +38539,7 @@
         <v>2.0296599999999998E-2</v>
       </c>
       <c r="J53" s="1">
-        <f>AVERAGE(F53:I53)</f>
+        <f t="shared" si="9"/>
         <v>2.0296749999999999E-2</v>
       </c>
     </row>
@@ -38522,19 +38548,19 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="B54" s="3">
-        <f>F54/$J54</f>
+        <f t="shared" si="5"/>
         <v>1.0000110857234359</v>
       </c>
       <c r="C54" s="3">
-        <f>G54/$J54</f>
+        <f t="shared" si="6"/>
         <v>1.0000012317470484</v>
       </c>
       <c r="D54" s="3">
-        <f>H54/$J54</f>
+        <f t="shared" si="7"/>
         <v>0.99999137777066116</v>
       </c>
       <c r="E54" s="3">
-        <f>I54/$J54</f>
+        <f t="shared" si="8"/>
         <v>0.99999630475885481</v>
       </c>
       <c r="F54" s="1">
@@ -38550,7 +38576,7 @@
         <v>2.02963E-2</v>
       </c>
       <c r="J54" s="1">
-        <f>AVERAGE(F54:I54)</f>
+        <f t="shared" si="9"/>
         <v>2.0296374999999998E-2</v>
       </c>
     </row>
@@ -38559,19 +38585,19 @@
         <v>2.6</v>
       </c>
       <c r="B55" s="3">
-        <f>F55/$J55</f>
+        <f t="shared" si="5"/>
         <v>1.0000123176677236</v>
       </c>
       <c r="C55" s="3">
-        <f>G55/$J55</f>
+        <f t="shared" si="6"/>
         <v>1.0000024635335447</v>
       </c>
       <c r="D55" s="3">
-        <f>H55/$J55</f>
+        <f t="shared" si="7"/>
         <v>0.99999260939936585</v>
       </c>
       <c r="E55" s="3">
-        <f>I55/$J55</f>
+        <f t="shared" si="8"/>
         <v>0.99999260939936585</v>
       </c>
       <c r="F55" s="1">
@@ -38587,7 +38613,7 @@
         <v>2.0295899999999999E-2</v>
       </c>
       <c r="J55" s="1">
-        <f>AVERAGE(F55:I55)</f>
+        <f t="shared" si="9"/>
         <v>2.029605E-2</v>
       </c>
     </row>
@@ -38596,19 +38622,19 @@
         <v>2.65</v>
       </c>
       <c r="B56" s="3">
-        <f>F56/$J56</f>
+        <f t="shared" si="5"/>
         <v>1.0000123178497962</v>
       </c>
       <c r="C56" s="3">
-        <f>G56/$J56</f>
+        <f t="shared" si="6"/>
         <v>1.0000024635699594</v>
       </c>
       <c r="D56" s="3">
-        <f>H56/$J56</f>
+        <f t="shared" si="7"/>
         <v>0.99999260929012246</v>
       </c>
       <c r="E56" s="3">
-        <f>I56/$J56</f>
+        <f t="shared" si="8"/>
         <v>0.99999260929012246</v>
       </c>
       <c r="F56" s="1">
@@ -38624,7 +38650,7 @@
         <v>2.02956E-2</v>
       </c>
       <c r="J56" s="1">
-        <f>AVERAGE(F56:I56)</f>
+        <f t="shared" si="9"/>
         <v>2.0295749999999998E-2</v>
       </c>
     </row>
@@ -38633,19 +38659,19 @@
         <v>2.7</v>
       </c>
       <c r="B57" s="3">
-        <f>F57/$J57</f>
+        <f t="shared" si="5"/>
         <v>1.000011086269655</v>
       </c>
       <c r="C57" s="3">
-        <f>G57/$J57</f>
+        <f t="shared" si="6"/>
         <v>1.0000012318077394</v>
       </c>
       <c r="D57" s="3">
-        <f>H57/$J57</f>
+        <f t="shared" si="7"/>
         <v>0.99999137734582377</v>
       </c>
       <c r="E57" s="3">
-        <f>I57/$J57</f>
+        <f t="shared" si="8"/>
         <v>0.99999630457678157</v>
       </c>
       <c r="F57" s="1">
@@ -38661,7 +38687,7 @@
         <v>2.0295299999999999E-2</v>
       </c>
       <c r="J57" s="1">
-        <f>AVERAGE(F57:I57)</f>
+        <f t="shared" si="9"/>
         <v>2.0295375000000001E-2</v>
       </c>
     </row>
@@ -38670,19 +38696,19 @@
         <v>2.75</v>
       </c>
       <c r="B58" s="3">
-        <f>F58/$J58</f>
+        <f t="shared" si="5"/>
         <v>1.000012318274653</v>
       </c>
       <c r="C58" s="3">
-        <f>G58/$J58</f>
+        <f t="shared" si="6"/>
         <v>1.0000024636549305</v>
       </c>
       <c r="D58" s="3">
-        <f>H58/$J58</f>
+        <f t="shared" si="7"/>
         <v>0.99999260903520804</v>
       </c>
       <c r="E58" s="3">
-        <f>I58/$J58</f>
+        <f t="shared" si="8"/>
         <v>0.99999260903520804</v>
       </c>
       <c r="F58" s="1">
@@ -38698,7 +38724,7 @@
         <v>2.0294900000000001E-2</v>
       </c>
       <c r="J58" s="1">
-        <f>AVERAGE(F58:I58)</f>
+        <f t="shared" si="9"/>
         <v>2.0295050000000002E-2</v>
       </c>
     </row>
@@ -38707,19 +38733,19 @@
         <v>2.8</v>
       </c>
       <c r="B59" s="3">
-        <f>F59/$J59</f>
+        <f t="shared" si="5"/>
         <v>1.0000123185174419</v>
       </c>
       <c r="C59" s="3">
-        <f>G59/$J59</f>
+        <f t="shared" si="6"/>
         <v>1.0000024637034883</v>
       </c>
       <c r="D59" s="3">
-        <f>H59/$J59</f>
+        <f t="shared" si="7"/>
         <v>0.9999926088895349</v>
       </c>
       <c r="E59" s="3">
-        <f>I59/$J59</f>
+        <f t="shared" si="8"/>
         <v>0.9999926088895349</v>
       </c>
       <c r="F59" s="1">
@@ -38735,7 +38761,7 @@
         <v>2.02945E-2</v>
       </c>
       <c r="J59" s="1">
-        <f>AVERAGE(F59:I59)</f>
+        <f t="shared" si="9"/>
         <v>2.0294650000000001E-2</v>
       </c>
     </row>
@@ -38744,19 +38770,19 @@
         <v>2.85</v>
       </c>
       <c r="B60" s="3">
-        <f>F60/$J60</f>
+        <f t="shared" si="5"/>
         <v>1.0000086231003003</v>
       </c>
       <c r="C60" s="3">
-        <f>G60/$J60</f>
+        <f t="shared" si="6"/>
         <v>1.0000036956144145</v>
       </c>
       <c r="D60" s="3">
-        <f>H60/$J60</f>
+        <f t="shared" si="7"/>
         <v>0.99999384064264274</v>
       </c>
       <c r="E60" s="3">
-        <f>I60/$J60</f>
+        <f t="shared" si="8"/>
         <v>0.99999384064264274</v>
       </c>
       <c r="F60" s="1">
@@ -38772,7 +38798,7 @@
         <v>2.0294199999999998E-2</v>
       </c>
       <c r="J60" s="1">
-        <f>AVERAGE(F60:I60)</f>
+        <f t="shared" si="9"/>
         <v>2.0294324999999998E-2</v>
       </c>
     </row>
@@ -38781,19 +38807,19 @@
         <v>2.9</v>
       </c>
       <c r="B61" s="3">
-        <f>F61/$J61</f>
+        <f t="shared" si="5"/>
         <v>1.0000110870344523</v>
       </c>
       <c r="C61" s="3">
-        <f>G61/$J61</f>
+        <f t="shared" si="6"/>
         <v>1.0000012318927169</v>
       </c>
       <c r="D61" s="3">
-        <f>H61/$J61</f>
+        <f t="shared" si="7"/>
         <v>0.9999913767509816</v>
       </c>
       <c r="E61" s="3">
-        <f>I61/$J61</f>
+        <f t="shared" si="8"/>
         <v>0.99999630432184927</v>
       </c>
       <c r="F61" s="1">
@@ -38809,7 +38835,7 @@
         <v>2.02939E-2</v>
       </c>
       <c r="J61" s="1">
-        <f>AVERAGE(F61:I61)</f>
+        <f t="shared" si="9"/>
         <v>2.0293974999999999E-2</v>
       </c>
     </row>
@@ -38818,19 +38844,19 @@
         <v>2.95</v>
       </c>
       <c r="B62" s="3">
-        <f>F62/$J62</f>
+        <f t="shared" si="5"/>
         <v>1.0000123191244552</v>
       </c>
       <c r="C62" s="3">
-        <f>G62/$J62</f>
+        <f t="shared" si="6"/>
         <v>1.0000024638248912</v>
       </c>
       <c r="D62" s="3">
-        <f>H62/$J62</f>
+        <f t="shared" si="7"/>
         <v>0.9999926085253269</v>
       </c>
       <c r="E62" s="3">
-        <f>I62/$J62</f>
+        <f t="shared" si="8"/>
         <v>0.9999926085253269</v>
       </c>
       <c r="F62" s="1">
@@ -38846,7 +38872,7 @@
         <v>2.0293499999999999E-2</v>
       </c>
       <c r="J62" s="1">
-        <f>AVERAGE(F62:I62)</f>
+        <f t="shared" si="9"/>
         <v>2.029365E-2</v>
       </c>
     </row>
@@ -38855,19 +38881,19 @@
         <v>3</v>
       </c>
       <c r="B63" s="3">
-        <f>F63/$J63</f>
+        <f t="shared" si="5"/>
         <v>1.0000123193672774</v>
       </c>
       <c r="C63" s="3">
-        <f>G63/$J63</f>
+        <f t="shared" si="6"/>
         <v>1.0000024638734555</v>
       </c>
       <c r="D63" s="3">
-        <f>H63/$J63</f>
+        <f t="shared" si="7"/>
         <v>0.99999260837963355</v>
       </c>
       <c r="E63" s="3">
-        <f>I63/$J63</f>
+        <f t="shared" si="8"/>
         <v>0.99999260837963355</v>
       </c>
       <c r="F63" s="1">
@@ -38883,7 +38909,7 @@
         <v>2.0293099999999998E-2</v>
       </c>
       <c r="J63" s="1">
-        <f>AVERAGE(F63:I63)</f>
+        <f t="shared" si="9"/>
         <v>2.0293249999999999E-2</v>
       </c>
     </row>
@@ -38892,19 +38918,19 @@
         <v>3.05</v>
       </c>
       <c r="B64" s="3">
-        <f>F64/$J64</f>
+        <f t="shared" si="5"/>
         <v>1.0000086236952039</v>
       </c>
       <c r="C64" s="3">
-        <f>G64/$J64</f>
+        <f t="shared" si="6"/>
         <v>1.0000036958693732</v>
       </c>
       <c r="D64" s="3">
-        <f>H64/$J64</f>
+        <f t="shared" si="7"/>
         <v>0.99999384021771132</v>
       </c>
       <c r="E64" s="3">
-        <f>I64/$J64</f>
+        <f t="shared" si="8"/>
         <v>0.99999384021771132</v>
       </c>
       <c r="F64" s="1">
@@ -38920,7 +38946,7 @@
         <v>2.02928E-2</v>
       </c>
       <c r="J64" s="1">
-        <f>AVERAGE(F64:I64)</f>
+        <f t="shared" si="9"/>
         <v>2.0292925E-2</v>
       </c>
     </row>
@@ -38929,19 +38955,19 @@
         <v>3.1</v>
       </c>
       <c r="B65" s="3">
-        <f>F65/$J65</f>
+        <f t="shared" si="5"/>
         <v>1.000012319792239</v>
       </c>
       <c r="C65" s="3">
-        <f>G65/$J65</f>
+        <f t="shared" si="6"/>
         <v>1.0000024639584479</v>
       </c>
       <c r="D65" s="3">
-        <f>H65/$J65</f>
+        <f t="shared" si="7"/>
         <v>0.99999260812465651</v>
       </c>
       <c r="E65" s="3">
-        <f>I65/$J65</f>
+        <f t="shared" si="8"/>
         <v>0.99999260812465651</v>
       </c>
       <c r="F65" s="1">
@@ -38957,7 +38983,7 @@
         <v>2.0292399999999999E-2</v>
       </c>
       <c r="J65" s="1">
-        <f>AVERAGE(F65:I65)</f>
+        <f t="shared" si="9"/>
         <v>2.0292549999999999E-2</v>
       </c>
     </row>
@@ -38966,19 +38992,19 @@
         <v>3.15</v>
       </c>
       <c r="B66" s="3">
-        <f>F66/$J66</f>
+        <f t="shared" si="5"/>
         <v>1.000011088017918</v>
       </c>
       <c r="C66" s="3">
-        <f>G66/$J66</f>
+        <f t="shared" si="6"/>
         <v>1.0000061600099543</v>
       </c>
       <c r="D66" s="3">
-        <f>H66/$J66</f>
+        <f t="shared" si="7"/>
         <v>0.99999137598606347</v>
       </c>
       <c r="E66" s="3">
-        <f>I66/$J66</f>
+        <f t="shared" si="8"/>
         <v>0.99999137598606347</v>
       </c>
       <c r="F66" s="1">
@@ -38994,7 +39020,7 @@
         <v>2.0292000000000001E-2</v>
       </c>
       <c r="J66" s="1">
-        <f>AVERAGE(F66:I66)</f>
+        <f t="shared" si="9"/>
         <v>2.0292175000000003E-2</v>
       </c>
     </row>
@@ -39003,19 +39029,19 @@
         <v>3.2</v>
       </c>
       <c r="B67" s="3">
-        <f>F67/$J67</f>
+        <f t="shared" ref="B67:B103" si="10">F67/$J67</f>
         <v>1.0000123202172302</v>
       </c>
       <c r="C67" s="3">
-        <f>G67/$J67</f>
+        <f t="shared" ref="C67:C103" si="11">G67/$J67</f>
         <v>1.0000024640434462</v>
       </c>
       <c r="D67" s="3">
-        <f>H67/$J67</f>
+        <f t="shared" ref="D67:D103" si="12">H67/$J67</f>
         <v>0.99999260786966204</v>
       </c>
       <c r="E67" s="3">
-        <f>I67/$J67</f>
+        <f t="shared" ref="E67:E103" si="13">I67/$J67</f>
         <v>0.99999260786966204</v>
       </c>
       <c r="F67" s="1">
@@ -39031,7 +39057,7 @@
         <v>2.0291699999999999E-2</v>
       </c>
       <c r="J67" s="1">
-        <f>AVERAGE(F67:I67)</f>
+        <f t="shared" ref="J67:J98" si="14">AVERAGE(F67:I67)</f>
         <v>2.0291849999999997E-2</v>
       </c>
     </row>
@@ -39040,19 +39066,19 @@
         <v>3.25</v>
       </c>
       <c r="B68" s="3">
-        <f>F68/$J68</f>
+        <f t="shared" si="10"/>
         <v>1.0000123204600952</v>
       </c>
       <c r="C68" s="3">
-        <f>G68/$J68</f>
+        <f t="shared" si="11"/>
         <v>1.0000024640920191</v>
       </c>
       <c r="D68" s="3">
-        <f>H68/$J68</f>
+        <f t="shared" si="12"/>
         <v>0.99999260772394283</v>
       </c>
       <c r="E68" s="3">
-        <f>I68/$J68</f>
+        <f t="shared" si="13"/>
         <v>0.99999260772394283</v>
       </c>
       <c r="F68" s="1">
@@ -39068,7 +39094,7 @@
         <v>2.0291299999999998E-2</v>
       </c>
       <c r="J68" s="1">
-        <f>AVERAGE(F68:I68)</f>
+        <f t="shared" si="14"/>
         <v>2.0291449999999999E-2</v>
       </c>
     </row>
@@ -39077,19 +39103,19 @@
         <v>3.3</v>
       </c>
       <c r="B69" s="3">
-        <f>F69/$J69</f>
+        <f t="shared" si="10"/>
         <v>1.0000098565380882</v>
       </c>
       <c r="C69" s="3">
-        <f>G69/$J69</f>
+        <f t="shared" si="11"/>
         <v>1.000004928269044</v>
       </c>
       <c r="D69" s="3">
-        <f>H69/$J69</f>
+        <f t="shared" si="12"/>
         <v>0.99999014346191195</v>
       </c>
       <c r="E69" s="3">
-        <f>I69/$J69</f>
+        <f t="shared" si="13"/>
         <v>0.99999507173095592</v>
       </c>
       <c r="F69" s="1">
@@ -39105,7 +39131,7 @@
         <v>2.0291E-2</v>
       </c>
       <c r="J69" s="1">
-        <f>AVERAGE(F69:I69)</f>
+        <f t="shared" si="14"/>
         <v>2.0291099999999999E-2</v>
       </c>
     </row>
@@ -39114,19 +39140,19 @@
         <v>3.35</v>
       </c>
       <c r="B70" s="3">
-        <f>F70/$J70</f>
+        <f t="shared" si="10"/>
         <v>1.0000086246302191</v>
       </c>
       <c r="C70" s="3">
-        <f>G70/$J70</f>
+        <f t="shared" si="11"/>
         <v>1.000003696270094</v>
       </c>
       <c r="D70" s="3">
-        <f>H70/$J70</f>
+        <f t="shared" si="12"/>
         <v>0.99999383954984356</v>
       </c>
       <c r="E70" s="3">
-        <f>I70/$J70</f>
+        <f t="shared" si="13"/>
         <v>0.99999383954984356</v>
       </c>
       <c r="F70" s="1">
@@ -39142,7 +39168,7 @@
         <v>2.0290599999999999E-2</v>
       </c>
       <c r="J70" s="1">
-        <f>AVERAGE(F70:I70)</f>
+        <f t="shared" si="14"/>
         <v>2.0290724999999999E-2</v>
       </c>
     </row>
@@ -39151,19 +39177,19 @@
         <v>3.4</v>
       </c>
       <c r="B71" s="3">
-        <f>F71/$J71</f>
+        <f t="shared" si="10"/>
         <v>1.0000123211280239</v>
       </c>
       <c r="C71" s="3">
-        <f>G71/$J71</f>
+        <f t="shared" si="11"/>
         <v>1.0000024642256049</v>
       </c>
       <c r="D71" s="3">
-        <f>H71/$J71</f>
+        <f t="shared" si="12"/>
         <v>0.99999260732318573</v>
       </c>
       <c r="E71" s="3">
-        <f>I71/$J71</f>
+        <f t="shared" si="13"/>
         <v>0.99999260732318573</v>
       </c>
       <c r="F71" s="1">
@@ -39179,7 +39205,7 @@
         <v>2.0290200000000001E-2</v>
       </c>
       <c r="J71" s="1">
-        <f>AVERAGE(F71:I71)</f>
+        <f t="shared" si="14"/>
         <v>2.0290349999999999E-2</v>
       </c>
     </row>
@@ -39188,19 +39214,19 @@
         <v>3.45</v>
       </c>
       <c r="B72" s="3">
-        <f>F72/$J72</f>
+        <f t="shared" si="10"/>
         <v>1.0000086249277662</v>
       </c>
       <c r="C72" s="3">
-        <f>G72/$J72</f>
+        <f t="shared" si="11"/>
         <v>1.000003696397614</v>
       </c>
       <c r="D72" s="3">
-        <f>H72/$J72</f>
+        <f t="shared" si="12"/>
         <v>0.99999383933730979</v>
       </c>
       <c r="E72" s="3">
-        <f>I72/$J72</f>
+        <f t="shared" si="13"/>
         <v>0.99999383933730979</v>
       </c>
       <c r="F72" s="1">
@@ -39216,7 +39242,7 @@
         <v>2.02899E-2</v>
       </c>
       <c r="J72" s="1">
-        <f>AVERAGE(F72:I72)</f>
+        <f t="shared" si="14"/>
         <v>2.0290025E-2</v>
       </c>
     </row>
@@ -39225,19 +39251,19 @@
         <v>3.5</v>
       </c>
       <c r="B73" s="3">
-        <f>F73/$J73</f>
+        <f t="shared" si="10"/>
         <v>1.0000123215531072</v>
       </c>
       <c r="C73" s="3">
-        <f>G73/$J73</f>
+        <f t="shared" si="11"/>
         <v>1.0000024643106216</v>
       </c>
       <c r="D73" s="3">
-        <f>H73/$J73</f>
+        <f t="shared" si="12"/>
         <v>0.99999260706813564</v>
       </c>
       <c r="E73" s="3">
-        <f>I73/$J73</f>
+        <f t="shared" si="13"/>
         <v>0.99999260706813564</v>
       </c>
       <c r="F73" s="1">
@@ -39253,7 +39279,7 @@
         <v>2.0289499999999999E-2</v>
       </c>
       <c r="J73" s="1">
-        <f>AVERAGE(F73:I73)</f>
+        <f t="shared" si="14"/>
         <v>2.0289649999999999E-2</v>
       </c>
     </row>
@@ -39262,19 +39288,19 @@
         <v>3.55</v>
       </c>
       <c r="B74" s="3">
-        <f>F74/$J74</f>
+        <f t="shared" si="10"/>
         <v>1.0000123217960248</v>
       </c>
       <c r="C74" s="3">
-        <f>G74/$J74</f>
+        <f t="shared" si="11"/>
         <v>1.0000024643592049</v>
       </c>
       <c r="D74" s="3">
-        <f>H74/$J74</f>
+        <f t="shared" si="12"/>
         <v>0.99999260692238501</v>
       </c>
       <c r="E74" s="3">
-        <f>I74/$J74</f>
+        <f t="shared" si="13"/>
         <v>0.99999260692238501</v>
       </c>
       <c r="F74" s="1">
@@ -39290,7 +39316,7 @@
         <v>2.0289100000000001E-2</v>
       </c>
       <c r="J74" s="1">
-        <f>AVERAGE(F74:I74)</f>
+        <f t="shared" si="14"/>
         <v>2.0289250000000002E-2</v>
       </c>
     </row>
@@ -39299,19 +39325,19 @@
         <v>3.6</v>
       </c>
       <c r="B75" s="3">
-        <f>F75/$J75</f>
+        <f t="shared" si="10"/>
         <v>1.0000123220389525</v>
       </c>
       <c r="C75" s="3">
-        <f>G75/$J75</f>
+        <f t="shared" si="11"/>
         <v>1.0000024644077903</v>
       </c>
       <c r="D75" s="3">
-        <f>H75/$J75</f>
+        <f t="shared" si="12"/>
         <v>0.99999260677662849</v>
       </c>
       <c r="E75" s="3">
-        <f>I75/$J75</f>
+        <f t="shared" si="13"/>
         <v>0.99999260677662849</v>
       </c>
       <c r="F75" s="1">
@@ -39327,7 +39353,7 @@
         <v>2.02887E-2</v>
       </c>
       <c r="J75" s="1">
-        <f>AVERAGE(F75:I75)</f>
+        <f t="shared" si="14"/>
         <v>2.0288850000000001E-2</v>
       </c>
     </row>
@@ -39336,19 +39362,19 @@
         <v>3.65</v>
       </c>
       <c r="B76" s="3">
-        <f>F76/$J76</f>
+        <f t="shared" si="10"/>
         <v>1.0000123222818895</v>
       </c>
       <c r="C76" s="3">
-        <f>G76/$J76</f>
+        <f t="shared" si="11"/>
         <v>1.0000024644563779</v>
       </c>
       <c r="D76" s="3">
-        <f>H76/$J76</f>
+        <f t="shared" si="12"/>
         <v>0.99999260663086631</v>
       </c>
       <c r="E76" s="3">
-        <f>I76/$J76</f>
+        <f t="shared" si="13"/>
         <v>0.99999260663086631</v>
       </c>
       <c r="F76" s="1">
@@ -39364,7 +39390,7 @@
         <v>2.0288299999999999E-2</v>
       </c>
       <c r="J76" s="1">
-        <f>AVERAGE(F76:I76)</f>
+        <f t="shared" si="14"/>
         <v>2.028845E-2</v>
       </c>
     </row>
@@ -39373,19 +39399,19 @@
         <v>3.7</v>
       </c>
       <c r="B77" s="3">
-        <f>F77/$J77</f>
+        <f t="shared" si="10"/>
         <v>1.0000098579955736</v>
       </c>
       <c r="C77" s="3">
-        <f>G77/$J77</f>
+        <f t="shared" si="11"/>
         <v>1.0000049289977868</v>
       </c>
       <c r="D77" s="3">
-        <f>H77/$J77</f>
+        <f t="shared" si="12"/>
         <v>0.99999014200442626</v>
       </c>
       <c r="E77" s="3">
-        <f>I77/$J77</f>
+        <f t="shared" si="13"/>
         <v>0.99999507100221319</v>
       </c>
       <c r="F77" s="1">
@@ -39401,7 +39427,7 @@
         <v>2.0288E-2</v>
       </c>
       <c r="J77" s="1">
-        <f>AVERAGE(F77:I77)</f>
+        <f t="shared" si="14"/>
         <v>2.02881E-2</v>
       </c>
     </row>
@@ -39410,19 +39436,19 @@
         <v>3.75</v>
       </c>
       <c r="B78" s="3">
-        <f>F78/$J78</f>
+        <f t="shared" si="10"/>
         <v>1.0000110904773465</v>
       </c>
       <c r="C78" s="3">
-        <f>G78/$J78</f>
+        <f t="shared" si="11"/>
         <v>1.0000012322752605</v>
       </c>
       <c r="D78" s="3">
-        <f>H78/$J78</f>
+        <f t="shared" si="12"/>
         <v>0.99999137407317484</v>
       </c>
       <c r="E78" s="3">
-        <f>I78/$J78</f>
+        <f t="shared" si="13"/>
         <v>0.99999630317421773</v>
       </c>
       <c r="F78" s="1">
@@ -39438,7 +39464,7 @@
         <v>2.0287599999999999E-2</v>
       </c>
       <c r="J78" s="1">
-        <f>AVERAGE(F78:I78)</f>
+        <f t="shared" si="14"/>
         <v>2.0287675000000002E-2</v>
       </c>
     </row>
@@ -39447,19 +39473,19 @@
         <v>3.8</v>
       </c>
       <c r="B79" s="3">
-        <f>F79/$J79</f>
+        <f t="shared" si="10"/>
         <v>1.000012323010758</v>
       </c>
       <c r="C79" s="3">
-        <f>G79/$J79</f>
+        <f t="shared" si="11"/>
         <v>1.0000024646021517</v>
       </c>
       <c r="D79" s="3">
-        <f>H79/$J79</f>
+        <f t="shared" si="12"/>
         <v>0.99999260619354513</v>
       </c>
       <c r="E79" s="3">
-        <f>I79/$J79</f>
+        <f t="shared" si="13"/>
         <v>0.99999260619354513</v>
       </c>
       <c r="F79" s="1">
@@ -39475,7 +39501,7 @@
         <v>2.0287099999999999E-2</v>
       </c>
       <c r="J79" s="1">
-        <f>AVERAGE(F79:I79)</f>
+        <f t="shared" si="14"/>
         <v>2.028725E-2</v>
       </c>
     </row>
@@ -39484,19 +39510,19 @@
         <v>3.85</v>
       </c>
       <c r="B80" s="3">
-        <f>F80/$J80</f>
+        <f t="shared" si="10"/>
         <v>1.0000123232537332</v>
       </c>
       <c r="C80" s="3">
-        <f>G80/$J80</f>
+        <f t="shared" si="11"/>
         <v>1.0000024646507466</v>
       </c>
       <c r="D80" s="3">
-        <f>H80/$J80</f>
+        <f t="shared" si="12"/>
         <v>0.99999260604775997</v>
       </c>
       <c r="E80" s="3">
-        <f>I80/$J80</f>
+        <f t="shared" si="13"/>
         <v>0.99999260604775997</v>
       </c>
       <c r="F80" s="1">
@@ -39512,7 +39538,7 @@
         <v>2.0286700000000001E-2</v>
       </c>
       <c r="J80" s="1">
-        <f>AVERAGE(F80:I80)</f>
+        <f t="shared" si="14"/>
         <v>2.0286850000000002E-2</v>
       </c>
     </row>
@@ -39521,19 +39547,19 @@
         <v>3.9</v>
       </c>
       <c r="B81" s="3">
-        <f>F81/$J81</f>
+        <f t="shared" si="10"/>
         <v>1.0000123234967182</v>
       </c>
       <c r="C81" s="3">
-        <f>G81/$J81</f>
+        <f t="shared" si="11"/>
         <v>1.0000024646993435</v>
       </c>
       <c r="D81" s="3">
-        <f>H81/$J81</f>
+        <f t="shared" si="12"/>
         <v>0.99999260590196903</v>
       </c>
       <c r="E81" s="3">
-        <f>I81/$J81</f>
+        <f t="shared" si="13"/>
         <v>0.99999260590196903</v>
       </c>
       <c r="F81" s="1">
@@ -39549,7 +39575,7 @@
         <v>2.02863E-2</v>
       </c>
       <c r="J81" s="1">
-        <f>AVERAGE(F81:I81)</f>
+        <f t="shared" si="14"/>
         <v>2.0286450000000001E-2</v>
       </c>
     </row>
@@ -39558,19 +39584,19 @@
         <v>3.95</v>
       </c>
       <c r="B82" s="3">
-        <f>F82/$J82</f>
+        <f t="shared" si="10"/>
         <v>1.0000098590160702</v>
       </c>
       <c r="C82" s="3">
-        <f>G82/$J82</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="D82" s="3">
-        <f>H82/$J82</f>
+        <f t="shared" si="12"/>
         <v>0.9999950704919649</v>
       </c>
       <c r="E82" s="3">
-        <f>I82/$J82</f>
+        <f t="shared" si="13"/>
         <v>0.9999950704919649</v>
       </c>
       <c r="F82" s="1">
@@ -39586,7 +39612,7 @@
         <v>2.0285899999999999E-2</v>
       </c>
       <c r="J82" s="1">
-        <f>AVERAGE(F82:I82)</f>
+        <f t="shared" si="14"/>
         <v>2.0285999999999998E-2</v>
       </c>
     </row>
@@ -39595,19 +39621,19 @@
         <v>4</v>
       </c>
       <c r="B83" s="3">
-        <f>F83/$J83</f>
+        <f t="shared" si="10"/>
         <v>1.0000110916801308</v>
       </c>
       <c r="C83" s="3">
-        <f>G83/$J83</f>
+        <f t="shared" si="11"/>
         <v>1.0000061620445171</v>
       </c>
       <c r="D83" s="3">
-        <f>H83/$J83</f>
+        <f t="shared" si="12"/>
         <v>0.99999137313767605</v>
       </c>
       <c r="E83" s="3">
-        <f>I83/$J83</f>
+        <f t="shared" si="13"/>
         <v>0.99999137313767605</v>
       </c>
       <c r="F83" s="1">
@@ -39623,7 +39649,7 @@
         <v>2.0285299999999999E-2</v>
       </c>
       <c r="J83" s="1">
-        <f>AVERAGE(F83:I83)</f>
+        <f t="shared" si="14"/>
         <v>2.0285475000000001E-2</v>
       </c>
     </row>
@@ -39632,19 +39658,19 @@
         <v>4.05</v>
       </c>
       <c r="B84" s="3">
-        <f>F84/$J84</f>
+        <f t="shared" si="10"/>
         <v>1.0000098595507003</v>
       </c>
       <c r="C84" s="3">
-        <f>G84/$J84</f>
+        <f t="shared" si="11"/>
         <v>1.0000049297753504</v>
       </c>
       <c r="D84" s="3">
-        <f>H84/$J84</f>
+        <f t="shared" si="12"/>
         <v>0.99999507022464984</v>
       </c>
       <c r="E84" s="3">
-        <f>I84/$J84</f>
+        <f t="shared" si="13"/>
         <v>0.99999014044929979</v>
       </c>
       <c r="F84" s="1">
@@ -39660,7 +39686,7 @@
         <v>2.0284699999999999E-2</v>
       </c>
       <c r="J84" s="1">
-        <f>AVERAGE(F84:I84)</f>
+        <f t="shared" si="14"/>
         <v>2.0284899999999998E-2</v>
       </c>
     </row>
@@ -39669,19 +39695,19 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B85" s="3">
-        <f>F85/$J85</f>
+        <f t="shared" si="10"/>
         <v>1.0000123249548289</v>
       </c>
       <c r="C85" s="3">
-        <f>G85/$J85</f>
+        <f t="shared" si="11"/>
         <v>1.0000024649909658</v>
       </c>
       <c r="D85" s="3">
-        <f>H85/$J85</f>
+        <f t="shared" si="12"/>
         <v>0.99999260502710274</v>
       </c>
       <c r="E85" s="3">
-        <f>I85/$J85</f>
+        <f t="shared" si="13"/>
         <v>0.99999260502710274</v>
       </c>
       <c r="F85" s="1">
@@ -39697,7 +39723,7 @@
         <v>2.0283900000000001E-2</v>
       </c>
       <c r="J85" s="1">
-        <f>AVERAGE(F85:I85)</f>
+        <f t="shared" si="14"/>
         <v>2.0284049999999998E-2</v>
       </c>
     </row>
@@ -39706,19 +39732,19 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="B86" s="3">
-        <f>F86/$J86</f>
+        <f t="shared" si="10"/>
         <v>1.0000135584028202</v>
       </c>
       <c r="C86" s="3">
-        <f>G86/$J86</f>
+        <f t="shared" si="11"/>
         <v>1.0000036977462239</v>
       </c>
       <c r="D86" s="3">
-        <f>H86/$J86</f>
+        <f t="shared" si="12"/>
         <v>0.99999383708962719</v>
       </c>
       <c r="E86" s="3">
-        <f>I86/$J86</f>
+        <f t="shared" si="13"/>
         <v>0.99998890676132901</v>
       </c>
       <c r="F86" s="1">
@@ -39734,7 +39760,7 @@
         <v>2.0282399999999999E-2</v>
       </c>
       <c r="J86" s="1">
-        <f>AVERAGE(F86:I86)</f>
+        <f t="shared" si="14"/>
         <v>2.0282624999999999E-2</v>
       </c>
     </row>
@@ -39743,19 +39769,19 @@
         <v>4.2</v>
       </c>
       <c r="B87" s="3">
-        <f>F87/$J87</f>
+        <f t="shared" si="10"/>
         <v>1.0000110944694069</v>
       </c>
       <c r="C87" s="3">
-        <f>G87/$J87</f>
+        <f t="shared" si="11"/>
         <v>1.0000061635941151</v>
       </c>
       <c r="D87" s="3">
-        <f>H87/$J87</f>
+        <f t="shared" si="12"/>
         <v>0.99999630184353105</v>
       </c>
       <c r="E87" s="3">
-        <f>I87/$J87</f>
+        <f t="shared" si="13"/>
         <v>0.9999864400929469</v>
       </c>
       <c r="F87" s="1">
@@ -39771,7 +39797,7 @@
         <v>2.0280099999999999E-2</v>
       </c>
       <c r="J87" s="1">
-        <f>AVERAGE(F87:I87)</f>
+        <f t="shared" si="14"/>
         <v>2.0280375E-2</v>
       </c>
     </row>
@@ -39780,19 +39806,19 @@
         <v>4.25</v>
       </c>
       <c r="B88" s="3">
-        <f>F88/$J88</f>
+        <f t="shared" si="10"/>
         <v>1.0000135621473072</v>
       </c>
       <c r="C88" s="3">
-        <f>G88/$J88</f>
+        <f t="shared" si="11"/>
         <v>1.0000086304573774</v>
       </c>
       <c r="D88" s="3">
-        <f>H88/$J88</f>
+        <f t="shared" si="12"/>
         <v>0.99999383538758779</v>
       </c>
       <c r="E88" s="3">
-        <f>I88/$J88</f>
+        <f t="shared" si="13"/>
         <v>0.99998397200772804</v>
       </c>
       <c r="F88" s="1">
@@ -39808,7 +39834,7 @@
         <v>2.0276699999999998E-2</v>
       </c>
       <c r="J88" s="1">
-        <f>AVERAGE(F88:I88)</f>
+        <f t="shared" si="14"/>
         <v>2.0277024999999997E-2</v>
       </c>
     </row>
@@ -39817,19 +39843,19 @@
         <v>4.3</v>
       </c>
       <c r="B89" s="3">
-        <f>F89/$J89</f>
+        <f t="shared" si="10"/>
         <v>1.0000160316687119</v>
       </c>
       <c r="C89" s="3">
-        <f>G89/$J89</f>
+        <f t="shared" si="11"/>
         <v>1.0000110988475697</v>
       </c>
       <c r="D89" s="3">
-        <f>H89/$J89</f>
+        <f t="shared" si="12"/>
         <v>0.99999630038414355</v>
       </c>
       <c r="E89" s="3">
-        <f>I89/$J89</f>
+        <f t="shared" si="13"/>
         <v>0.99997656909957522</v>
       </c>
       <c r="F89" s="1">
@@ -39845,7 +39871,7 @@
         <v>2.0271899999999999E-2</v>
       </c>
       <c r="J89" s="1">
-        <f>AVERAGE(F89:I89)</f>
+        <f t="shared" si="14"/>
         <v>2.0272374999999999E-2</v>
       </c>
     </row>
@@ -39854,19 +39880,19 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="B90" s="3">
-        <f>F90/$J90</f>
+        <f t="shared" si="10"/>
         <v>1.0000185036927203</v>
       </c>
       <c r="C90" s="3">
-        <f>G90/$J90</f>
+        <f t="shared" si="11"/>
         <v>1.0000135693746617</v>
       </c>
       <c r="D90" s="3">
-        <f>H90/$J90</f>
+        <f t="shared" si="12"/>
         <v>0.99999383210242654</v>
       </c>
       <c r="E90" s="3">
-        <f>I90/$J90</f>
+        <f t="shared" si="13"/>
         <v>0.99997409483019173</v>
       </c>
       <c r="F90" s="1">
@@ -39882,7 +39908,7 @@
         <v>2.0265700000000001E-2</v>
       </c>
       <c r="J90" s="1">
-        <f>AVERAGE(F90:I90)</f>
+        <f t="shared" si="14"/>
         <v>2.0266224999999999E-2</v>
       </c>
     </row>
@@ -39891,19 +39917,19 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B91" s="3">
-        <f>F91/$J91</f>
+        <f t="shared" si="10"/>
         <v>1.0000209786671634</v>
       </c>
       <c r="C91" s="3">
-        <f>G91/$J91</f>
+        <f t="shared" si="11"/>
         <v>1.0000160425101838</v>
       </c>
       <c r="D91" s="3">
-        <f>H91/$J91</f>
+        <f t="shared" si="12"/>
         <v>0.99999629788226518</v>
       </c>
       <c r="E91" s="3">
-        <f>I91/$J91</f>
+        <f t="shared" si="13"/>
         <v>0.99996668094038721</v>
       </c>
       <c r="F91" s="1">
@@ -39919,7 +39945,7 @@
         <v>2.0257999999999998E-2</v>
       </c>
       <c r="J91" s="1">
-        <f>AVERAGE(F91:I91)</f>
+        <f t="shared" si="14"/>
         <v>2.0258675E-2</v>
       </c>
     </row>
@@ -39928,19 +39954,19 @@
         <v>4.45</v>
       </c>
       <c r="B92" s="3">
-        <f>F92/$J92</f>
+        <f t="shared" si="10"/>
         <v>1.0000222227160602</v>
       </c>
       <c r="C92" s="3">
-        <f>G92/$J92</f>
+        <f t="shared" si="11"/>
         <v>1.0000172843347135</v>
       </c>
       <c r="D92" s="3">
-        <f>H92/$J92</f>
+        <f t="shared" si="12"/>
         <v>0.99999753080932652</v>
       </c>
       <c r="E92" s="3">
-        <f>I92/$J92</f>
+        <f t="shared" si="13"/>
         <v>0.99996296213989933</v>
       </c>
       <c r="F92" s="1">
@@ -39956,7 +39982,7 @@
         <v>2.0248800000000001E-2</v>
       </c>
       <c r="J92" s="1">
-        <f>AVERAGE(F92:I92)</f>
+        <f t="shared" si="14"/>
         <v>2.0249550000000002E-2</v>
       </c>
     </row>
@@ -39965,19 +39991,19 @@
         <v>4.5</v>
       </c>
       <c r="B93" s="3">
-        <f>F93/$J93</f>
+        <f t="shared" si="10"/>
         <v>1.0000296479308215</v>
       </c>
       <c r="C93" s="3">
-        <f>G93/$J93</f>
+        <f t="shared" si="11"/>
         <v>1.0000197652872145</v>
       </c>
       <c r="D93" s="3">
-        <f>H93/$J93</f>
+        <f t="shared" si="12"/>
         <v>0.99999505867819649</v>
       </c>
       <c r="E93" s="3">
-        <f>I93/$J93</f>
+        <f t="shared" si="13"/>
         <v>0.99995552810376787</v>
       </c>
       <c r="F93" s="1">
@@ -39993,7 +40019,7 @@
         <v>2.02366E-2</v>
       </c>
       <c r="J93" s="1">
-        <f>AVERAGE(F93:I93)</f>
+        <f t="shared" si="14"/>
         <v>2.0237499999999999E-2</v>
       </c>
     </row>
@@ -40002,19 +40028,19 @@
         <v>4.55</v>
       </c>
       <c r="B94" s="3">
-        <f>F94/$J94</f>
+        <f t="shared" si="10"/>
         <v>1.0000482266802362</v>
       </c>
       <c r="C94" s="3">
-        <f>G94/$J94</f>
+        <f t="shared" si="11"/>
         <v>1.0000284413755238</v>
       </c>
       <c r="D94" s="3">
-        <f>H94/$J94</f>
+        <f t="shared" si="12"/>
         <v>0.99999381709227741</v>
       </c>
       <c r="E94" s="3">
-        <f>I94/$J94</f>
+        <f t="shared" si="13"/>
         <v>0.99992951485196269</v>
       </c>
       <c r="F94" s="1">
@@ -40030,7 +40056,7 @@
         <v>2.02156E-2</v>
       </c>
       <c r="J94" s="1">
-        <f>AVERAGE(F94:I94)</f>
+        <f t="shared" si="14"/>
         <v>2.0217025E-2</v>
       </c>
     </row>
@@ -40039,19 +40065,19 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="B95" s="3">
-        <f>F95/$J95</f>
+        <f t="shared" si="10"/>
         <v>1.0000780795891278</v>
       </c>
       <c r="C95" s="3">
-        <f>G95/$J95</f>
+        <f t="shared" si="11"/>
         <v>1.0000780795891278</v>
       </c>
       <c r="D95" s="3">
-        <f>H95/$J95</f>
+        <f t="shared" si="12"/>
         <v>1.0000086755099031</v>
       </c>
       <c r="E95" s="3">
-        <f>I95/$J95</f>
+        <f t="shared" si="13"/>
         <v>0.99983516531184125</v>
       </c>
       <c r="F95" s="1">
@@ -40067,7 +40093,7 @@
         <v>2.01684E-2</v>
       </c>
       <c r="J95" s="1">
-        <f>AVERAGE(F95:I95)</f>
+        <f t="shared" si="14"/>
         <v>2.0171724999999998E-2</v>
       </c>
     </row>
@@ -40076,19 +40102,19 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="B96" s="3">
-        <f>F96/$J96</f>
+        <f t="shared" si="10"/>
         <v>1.000149603550591</v>
       </c>
       <c r="C96" s="3">
-        <f>G96/$J96</f>
+        <f t="shared" si="11"/>
         <v>1.0001994714007878</v>
       </c>
       <c r="D96" s="3">
-        <f>H96/$J96</f>
+        <f t="shared" si="12"/>
         <v>1.0000498678501968</v>
       </c>
       <c r="E96" s="3">
-        <f>I96/$J96</f>
+        <f t="shared" si="13"/>
         <v>0.99960105719842407</v>
       </c>
       <c r="F96" s="1">
@@ -40104,7 +40130,7 @@
         <v>2.0045E-2</v>
       </c>
       <c r="J96" s="1">
-        <f>AVERAGE(F96:I96)</f>
+        <f t="shared" si="14"/>
         <v>2.0053000000000001E-2</v>
       </c>
     </row>
@@ -40113,19 +40139,19 @@
         <v>4.7</v>
       </c>
       <c r="B97" s="3">
-        <f>F97/$J97</f>
+        <f t="shared" si="10"/>
         <v>1.0002650477717057</v>
       </c>
       <c r="C97" s="3">
-        <f>G97/$J97</f>
+        <f t="shared" si="11"/>
         <v>1.0004669889311004</v>
       </c>
       <c r="D97" s="3">
-        <f>H97/$J97</f>
+        <f t="shared" si="12"/>
         <v>1.0001135919021595</v>
       </c>
       <c r="E97" s="3">
-        <f>I97/$J97</f>
+        <f t="shared" si="13"/>
         <v>0.99915437139503482</v>
       </c>
       <c r="F97" s="1">
@@ -40141,7 +40167,7 @@
         <v>1.9791E-2</v>
       </c>
       <c r="J97" s="1">
-        <f>AVERAGE(F97:I97)</f>
+        <f t="shared" si="14"/>
         <v>1.9807749999999999E-2</v>
       </c>
     </row>
@@ -40150,19 +40176,19 @@
         <v>4.75</v>
       </c>
       <c r="B98" s="3">
-        <f>F98/$J98</f>
+        <f t="shared" si="10"/>
         <v>1.0003871067640455</v>
       </c>
       <c r="C98" s="3">
-        <f>G98/$J98</f>
+        <f t="shared" si="11"/>
         <v>1.0008516348809</v>
       </c>
       <c r="D98" s="3">
-        <f>H98/$J98</f>
+        <f t="shared" si="12"/>
         <v>1.000129035588015</v>
       </c>
       <c r="E98" s="3">
-        <f>I98/$J98</f>
+        <f t="shared" si="13"/>
         <v>0.99863222276703922</v>
       </c>
       <c r="F98" s="1">
@@ -40178,7 +40204,7 @@
         <v>1.9348000000000001E-2</v>
       </c>
       <c r="J98" s="1">
-        <f>AVERAGE(F98:I98)</f>
+        <f t="shared" si="14"/>
         <v>1.9374499999999999E-2</v>
       </c>
     </row>
@@ -40187,19 +40213,19 @@
         <v>4.8</v>
       </c>
       <c r="B99" s="3">
-        <f>F99/$J99</f>
+        <f t="shared" si="10"/>
         <v>1.0004656174752891</v>
       </c>
       <c r="C99" s="3">
-        <f>G99/$J99</f>
+        <f t="shared" si="11"/>
         <v>1.0010509651585096</v>
       </c>
       <c r="D99" s="3">
-        <f>H99/$J99</f>
+        <f t="shared" si="12"/>
         <v>1.0003059771980471</v>
       </c>
       <c r="E99" s="3">
-        <f>I99/$J99</f>
+        <f t="shared" si="13"/>
         <v>0.99817744016815468</v>
       </c>
       <c r="F99" s="1">
@@ -40215,7 +40241,7 @@
         <v>1.8758E-2</v>
       </c>
       <c r="J99" s="1">
-        <f>AVERAGE(F99:I99)</f>
+        <f t="shared" ref="J99:J130" si="15">AVERAGE(F99:I99)</f>
         <v>1.8792249999999996E-2</v>
       </c>
     </row>
@@ -40224,19 +40250,19 @@
         <v>4.8499999999999996</v>
       </c>
       <c r="B100" s="3">
-        <f>F100/$J100</f>
+        <f t="shared" si="10"/>
         <v>1.0004161464835621</v>
       </c>
       <c r="C100" s="3">
-        <f>G100/$J100</f>
+        <f t="shared" si="11"/>
         <v>1.0015258704397281</v>
       </c>
       <c r="D100" s="3">
-        <f>H100/$J100</f>
+        <f t="shared" si="12"/>
         <v>1.0004161464835621</v>
       </c>
       <c r="E100" s="3">
-        <f>I100/$J100</f>
+        <f t="shared" si="13"/>
         <v>0.99764183659314742</v>
       </c>
       <c r="F100" s="1">
@@ -40252,7 +40278,7 @@
         <v>1.7979999999999999E-2</v>
       </c>
       <c r="J100" s="1">
-        <f>AVERAGE(F100:I100)</f>
+        <f t="shared" si="15"/>
         <v>1.80225E-2</v>
       </c>
     </row>
@@ -40261,19 +40287,19 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="B101" s="3">
-        <f>F101/$J101</f>
+        <f t="shared" si="10"/>
         <v>1.0008683068017368</v>
       </c>
       <c r="C101" s="3">
-        <f>G101/$J101</f>
+        <f t="shared" si="11"/>
         <v>1.0014471780028944</v>
       </c>
       <c r="D101" s="3">
-        <f>H101/$J101</f>
+        <f t="shared" si="12"/>
         <v>1.0002894356005789</v>
       </c>
       <c r="E101" s="3">
-        <f>I101/$J101</f>
+        <f t="shared" si="13"/>
         <v>0.99739507959479012</v>
       </c>
       <c r="F101" s="1">
@@ -40289,7 +40315,7 @@
         <v>1.7229999999999999E-2</v>
       </c>
       <c r="J101" s="1">
-        <f>AVERAGE(F101:I101)</f>
+        <f t="shared" si="15"/>
         <v>1.7274999999999999E-2</v>
       </c>
     </row>
@@ -40298,19 +40324,19 @@
         <v>4.95</v>
       </c>
       <c r="B102" s="3">
-        <f>F102/$J102</f>
+        <f t="shared" si="10"/>
         <v>1.0007586102260657</v>
       </c>
       <c r="C102" s="3">
-        <f>G102/$J102</f>
+        <f t="shared" si="11"/>
         <v>1.0013654984069187</v>
       </c>
       <c r="D102" s="3">
-        <f>H102/$J102</f>
+        <f t="shared" si="12"/>
         <v>1.0007586102260657</v>
       </c>
       <c r="E102" s="3">
-        <f>I102/$J102</f>
+        <f t="shared" si="13"/>
         <v>0.99711728114094988</v>
       </c>
       <c r="F102" s="1">
@@ -40326,7 +40352,7 @@
         <v>1.643E-2</v>
       </c>
       <c r="J102" s="1">
-        <f>AVERAGE(F102:I102)</f>
+        <f t="shared" si="15"/>
         <v>1.6477499999999999E-2</v>
       </c>
     </row>
@@ -40335,19 +40361,19 @@
         <v>5</v>
       </c>
       <c r="B103" s="3">
-        <f>F103/$J103</f>
+        <f t="shared" si="10"/>
         <v>1.0012787723785168</v>
       </c>
       <c r="C103" s="3">
-        <f>G103/$J103</f>
+        <f t="shared" si="11"/>
         <v>1.001918158567775</v>
       </c>
       <c r="D103" s="3">
-        <f>H103/$J103</f>
+        <f t="shared" si="12"/>
         <v>1.0006393861892584</v>
       </c>
       <c r="E103" s="3">
-        <f>I103/$J103</f>
+        <f t="shared" si="13"/>
         <v>0.99616368286445023</v>
       </c>
       <c r="F103" s="1">
@@ -40363,7 +40389,7 @@
         <v>1.558E-2</v>
       </c>
       <c r="J103" s="1">
-        <f>AVERAGE(F103:I103)</f>
+        <f t="shared" si="15"/>
         <v>1.5639999999999998E-2</v>
       </c>
     </row>
@@ -40375,15 +40401,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:Q103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -40392,7 +40422,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -40423,8 +40453,26 @@
       <c r="J2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -40455,8 +40503,31 @@
       <c r="J3" s="1">
         <v>6.9999999999999996E-10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3">
+        <f>1.58*(10^(-12))</f>
+        <v>1.5800000000000001E-12</v>
+      </c>
+      <c r="N3">
+        <f>1.922*(10^(-12))</f>
+        <v>1.9220000000000001E-12</v>
+      </c>
+      <c r="O3">
+        <f>1.824*(10^(-12))</f>
+        <v>1.8239999999999999E-12</v>
+      </c>
+      <c r="P3">
+        <f>2.798*(10^(-12))</f>
+        <v>2.798E-12</v>
+      </c>
+      <c r="Q3">
+        <f>AVERAGE(M3:P3)</f>
+        <v>2.0310000000000001E-12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.05</v>
       </c>
@@ -40487,8 +40558,31 @@
       <c r="J4" s="1">
         <v>6.9999999999999996E-10</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4">
+        <f>M3/$Q$3</f>
+        <v>0.77794190054160517</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:P4" si="0">N3/$Q$3</f>
+        <v>0.94633185622845883</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0.89807976366321995</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>1.3776464795667158</v>
+      </c>
+      <c r="Q4">
+        <f>Q3/$Q$3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.1</v>
       </c>
@@ -40519,8 +40613,28 @@
       <c r="J5" s="1">
         <v>1.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f>(M4-1)*100</f>
+        <v>-22.205809945839484</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:Q5" si="1">(N4-1)*100</f>
+        <v>-5.3668143771541166</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>-10.192023633678005</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>37.764647956671581</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.15</v>
       </c>
@@ -40552,7 +40666,7 @@
         <v>2.7000000000000002E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.2</v>
       </c>
@@ -40584,7 +40698,7 @@
         <v>1.5399999999999999E-8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.25</v>
       </c>
@@ -40616,7 +40730,7 @@
         <v>1.034E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.3</v>
       </c>
@@ -40648,7 +40762,7 @@
         <v>7.1800000000000005E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.35</v>
       </c>
@@ -40680,7 +40794,7 @@
         <v>4.8899999999999998E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.4</v>
       </c>
@@ -40712,7 +40826,7 @@
         <v>2.037E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.45</v>
       </c>
@@ -40744,7 +40858,7 @@
         <v>2.3000000000000001E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.5</v>
       </c>
@@ -40776,7 +40890,7 @@
         <v>1.6659999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.55000000000000004</v>
       </c>
@@ -40808,7 +40922,7 @@
         <v>1.0410000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.6</v>
       </c>
@@ -40840,7 +40954,7 @@
         <v>2.036E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.65</v>
       </c>
@@ -42558,7 +42672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
@@ -48181,7 +48295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F13" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>